<commit_message>
When the attachment file is too long, shutil move will fail. So we will cut file name if it exceed 60 character
</commit_message>
<xml_diff>
--- a/New Products Assmt.xlsx
+++ b/New Products Assmt.xlsx
@@ -1,20 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wahyu\PT Telekomunikasi Selular\muhammad_f_rais - POSTPAID REVAS onedrive\New Products Assurance\2019-02\email\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="10" documentId="114_{A497BF04-5BFF-4F7D-8CF1-BD4341CAC932}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{046F0ED7-98A8-446E-8BCF-E462351BC267}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="194">
   <si>
     <t>No</t>
   </si>
@@ -28,6 +42,9 @@
     <t>Tanggal Terima</t>
   </si>
   <si>
+    <t>Tanggal Close</t>
+  </si>
+  <si>
     <t>Assessment Status</t>
   </si>
   <si>
@@ -259,6 +276,45 @@
     <t>028/MK.05/PS-03/II/2019</t>
   </si>
   <si>
+    <t>033/MK.05/PS-33/II/2019</t>
+  </si>
+  <si>
+    <t>029/MK.05/PS-03/II/2019</t>
+  </si>
+  <si>
+    <t>037/MK.05/PS-33/II/2019</t>
+  </si>
+  <si>
+    <t>0192/MK.05/PS-05/II/2019</t>
+  </si>
+  <si>
+    <t>032/MK.05/PS-03/II/2019</t>
+  </si>
+  <si>
+    <t>031/MK.05/PS-03/II/2019</t>
+  </si>
+  <si>
+    <t>0197/MK.05/PS-05/II/2019</t>
+  </si>
+  <si>
+    <t>042/MK.05/PS-33/II/2019</t>
+  </si>
+  <si>
+    <t>034/MK.05/PS-03/II/2019</t>
+  </si>
+  <si>
+    <t>0208/MK.05/PS-05/II/2019</t>
+  </si>
+  <si>
+    <t>027/MK.05/PS-37/II/2019</t>
+  </si>
+  <si>
+    <t>016/SV.05/CM-61/II/2019</t>
+  </si>
+  <si>
+    <t>017/SV.05/CM-61/II/2019</t>
+  </si>
+  <si>
     <t>[Nota Dinas] Permohonan Batch Offer untuk Pelanggan BC 06 per Januari 2019 (005/MK.05/PS-03/I/2019)</t>
   </si>
   <si>
@@ -478,6 +534,45 @@
     <t>FW: [Nota Dinas] Permohonan Batch Upgrade CLS Domestik Pelanggan kartuHALO (028/MK.05/PS-03/II/2019)</t>
   </si>
   <si>
+    <t>[Nota Dinas] Pemberitahuan RFI Penambahan Coverage Paket Roaming Promo Eropa Amerika (Voice &amp;amp; SMS) (033/MK.05/PS-33/II/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Permohonan Batch Offer untuk Pelanggan BC 11 per Februari 2019 (029/MK.05/PS-03/II/2019)</t>
+  </si>
+  <si>
+    <t>FW: [Nota Dinas] Pemberitahuan RFS Paket Roamazing (037/MK.05/PS-33/II/2019)</t>
+  </si>
+  <si>
+    <t>FW: [Nota Dinas] Status Kesiapan Komersial (RFC) FO Device Installment Corporate W3 Feb (0192/MK.05/PS-05/II/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Permohonan Batch Offer Bonus Spesial Migrasi (032/MK.05/PS-03/II/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Permohonan Batch Value CLS (031/MK.05/PS-03/II/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Status Kesiapan Komersial (RFC) Weekend Voice Deal pada sistem Digicore (0197/MK.05/PS-05/II/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFS Paket Roaming Prepaid Standalone pada Sistem Digicore (Promo Eropa Amerika, Asia Reguler, Eropa Reguler, Amerika Afrika, dan Haji) (042/MK.05/PS-33/II/2019)</t>
+  </si>
+  <si>
+    <t>FW: [Nota Dinas] Permohonan Batch Perubahan CLS Domestik Pelanggan kartuHALO Menjadi Rp500,000 (034/MK.05/PS-03/II/2019)</t>
+  </si>
+  <si>
+    <t>FW: [Nota Dinas] Status Kesiapan Komersial (RFC)  Paket Project PT. Akses Prima Indonesia Postpaid (0208/MK.05/PS-05/II/2019)</t>
+  </si>
+  <si>
+    <t>FW: [Nota Dinas] Pemberitahuan RFS Halo Kick Bundling Samsung S10 (027/MK.05/PS-37/II/2019)</t>
+  </si>
+  <si>
+    <t>FW: [Nota Dinas] Permohonan Migration APN Corporate Legacy KEMENKEU Menjadi M2M (016/SV.05/CM-61/II/2019)</t>
+  </si>
+  <si>
+    <t>FW: [Nota Dinas] Permohonan Migration APN Corporate Legacy KEMENKEU Menjadi M2M (017/SV.05/CM-61/II/2019)</t>
+  </si>
+  <si>
     <t>in progress</t>
   </si>
   <si>
@@ -503,16 +598,28 @@
   </si>
   <si>
     <t>Konfirmasi perubahan behaviour paket roaming, dimana sebelumnya bersifat akumulatif menjadi terpisah per paket. Mekanisme charging sama persis dg sebelum perubahan. Tiap customer disediakan bucket packet 5 sd 15 bucket.</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Status Kesiapan Komersial (RFC) Paket Promo Roaming Eropa dan Amerika di B2B2C (1 dan 30 Hari Internet &amp;amp;3in1).pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0214/MK.05/PS-05/II/2019 </t>
+  </si>
+  <si>
+    <t>48 - Sosialisasi Program Quick Win Family Plan</t>
+  </si>
+  <si>
+    <t>048/MK.05/MK-01/II/2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -576,6 +683,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -622,7 +737,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -654,9 +769,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -688,6 +821,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -863,14 +1014,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -895,1270 +1051,1528 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="D2" s="2">
         <v>43480</v>
       </c>
-      <c r="E2" t="s">
-        <v>154</v>
-      </c>
       <c r="F2" t="s">
-        <v>156</v>
-      </c>
-      <c r="H2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>181</v>
+      </c>
+      <c r="G2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D3" s="2">
         <v>43480</v>
       </c>
-      <c r="E3" t="s">
-        <v>154</v>
-      </c>
       <c r="F3" t="s">
-        <v>157</v>
-      </c>
-      <c r="H3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>181</v>
+      </c>
+      <c r="G3" t="s">
+        <v>184</v>
+      </c>
+      <c r="I3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="D4" s="2">
         <v>43481</v>
       </c>
-      <c r="E4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="F4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="D5" s="2">
         <v>43481</v>
       </c>
-      <c r="E5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="F5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="D6" s="2">
         <v>43483</v>
       </c>
-      <c r="E6" t="s">
-        <v>155</v>
-      </c>
-      <c r="H6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="F6" t="s">
+        <v>182</v>
+      </c>
+      <c r="I6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="D7" s="2">
         <v>43487</v>
       </c>
-      <c r="E7" t="s">
-        <v>155</v>
-      </c>
       <c r="F7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>182</v>
+      </c>
+      <c r="G7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D8" s="2">
         <v>43493</v>
       </c>
-      <c r="E8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="F8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="D9" s="2">
         <v>43510</v>
       </c>
-      <c r="E9" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="F9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D10" s="2">
         <v>43510</v>
       </c>
-      <c r="E10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="F10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="D11" s="2">
         <v>43510</v>
       </c>
-      <c r="E11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="F11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="D12" s="2">
         <v>43510</v>
       </c>
-      <c r="E12" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="F12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="D13" s="2">
         <v>43510</v>
       </c>
-      <c r="E13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="F13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="D14" s="2">
         <v>43510</v>
       </c>
-      <c r="E14" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="F14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="D15" s="2">
         <v>43510</v>
       </c>
-      <c r="E15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="F15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="D16" s="2">
         <v>43510</v>
       </c>
-      <c r="E16" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="D17" s="2">
         <v>43510</v>
       </c>
-      <c r="E17" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="D18" s="2">
         <v>43510</v>
       </c>
-      <c r="E18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="D19" s="2">
         <v>43510</v>
       </c>
-      <c r="E19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="D20" s="2">
         <v>43510</v>
       </c>
-      <c r="E20" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="D21" s="2">
         <v>43510</v>
       </c>
-      <c r="E21" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="D22" s="2">
         <v>43510</v>
       </c>
-      <c r="E22" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="D23" s="2">
         <v>43510</v>
       </c>
-      <c r="E23" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="D24" s="2">
         <v>43510</v>
       </c>
-      <c r="E24" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="D25" s="2">
         <v>43510</v>
       </c>
-      <c r="E25" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="D26" s="2">
         <v>43510</v>
       </c>
-      <c r="E26" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="D27" s="2">
         <v>43510</v>
       </c>
-      <c r="E27" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="D28" s="2">
         <v>43510</v>
       </c>
-      <c r="E28" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="D29" s="2">
         <v>43510</v>
       </c>
-      <c r="E29" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="D30" s="2">
         <v>43510</v>
       </c>
-      <c r="E30" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="D31" s="2">
         <v>43510</v>
       </c>
-      <c r="E31" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="D32" s="2">
         <v>43510</v>
       </c>
-      <c r="E32" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="F32" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="D33" s="2">
         <v>43510</v>
       </c>
-      <c r="E33" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="F33" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="D34" s="2">
         <v>43510</v>
       </c>
-      <c r="E34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="F34" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="D35" s="2">
         <v>43510</v>
       </c>
-      <c r="E35" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="F35" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="D36" s="2">
         <v>43510</v>
       </c>
-      <c r="E36" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="F36" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="D37" s="2">
         <v>43510</v>
       </c>
-      <c r="E37" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="F37" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="D38" s="2">
         <v>43511</v>
       </c>
-      <c r="E38" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="F38" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C39" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="D39" s="2">
         <v>43511</v>
       </c>
-      <c r="E39" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="F39" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="D40" s="2">
         <v>43511</v>
       </c>
-      <c r="E40" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="F40" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="D41" s="2">
         <v>43511</v>
       </c>
-      <c r="E41" t="s">
-        <v>154</v>
-      </c>
       <c r="F41" t="s">
-        <v>158</v>
-      </c>
-      <c r="H41" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>181</v>
+      </c>
+      <c r="G41" t="s">
+        <v>185</v>
+      </c>
+      <c r="I41" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="D42" s="2">
         <v>43511</v>
       </c>
-      <c r="E42" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="F42" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="D43" s="2">
         <v>43511</v>
       </c>
-      <c r="E43" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="F43" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="D44" s="2">
         <v>43511</v>
       </c>
-      <c r="E44" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="F44" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C45" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="D45" s="2">
         <v>43511</v>
       </c>
-      <c r="E45" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="F45" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="D46" s="2">
         <v>43511</v>
       </c>
-      <c r="E46" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="F46" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C47" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="D47" s="2">
         <v>43511</v>
       </c>
-      <c r="E47" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="F47" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C48" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="D48" s="2">
         <v>43511</v>
       </c>
-      <c r="E48" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>41</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="D49" s="2">
         <v>43511</v>
       </c>
-      <c r="E49" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>42</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C50" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="D50" s="2">
         <v>43511</v>
       </c>
-      <c r="E50" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="D51" s="2">
         <v>43511</v>
       </c>
-      <c r="E51" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C52" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="D52" s="2">
         <v>43511</v>
       </c>
-      <c r="E52" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>45</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C53" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="D53" s="2">
         <v>43511</v>
       </c>
-      <c r="E53" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>46</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="D54" s="2">
         <v>43511</v>
       </c>
-      <c r="E54" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>47</v>
       </c>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="D55" s="2">
         <v>43511</v>
       </c>
-      <c r="E55" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>48</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="D56" s="2">
         <v>43511</v>
       </c>
-      <c r="E56" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>49</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C57" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="D57" s="2">
         <v>43511</v>
       </c>
-      <c r="E57" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>50</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D58" s="2">
         <v>43511</v>
       </c>
-      <c r="E58" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>51</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C59" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="D59" s="2">
         <v>43511</v>
       </c>
-      <c r="E59" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>52</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C60" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="D60" s="2">
         <v>43511</v>
       </c>
-      <c r="E60" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>53</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C61" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="D61" s="2">
         <v>43511</v>
       </c>
-      <c r="E61" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>54</v>
       </c>
       <c r="B62" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C62" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="D62" s="2">
         <v>43511</v>
       </c>
-      <c r="E62" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>55</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C63" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="D63" s="2">
         <v>43511</v>
       </c>
-      <c r="E63" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>56</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C64" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="D64" s="2">
         <v>43511</v>
       </c>
-      <c r="E64" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>57</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="D65" s="2">
         <v>43511</v>
       </c>
-      <c r="E65" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>58</v>
       </c>
       <c r="B66" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C66" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="D66" s="2">
         <v>43511</v>
       </c>
-      <c r="E66" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="F66" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>59</v>
       </c>
       <c r="B67" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C67" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="D67" s="2">
         <v>43511</v>
       </c>
-      <c r="E67" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="F67" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>60</v>
       </c>
       <c r="B68" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C68" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="D68" s="2">
         <v>43511</v>
       </c>
-      <c r="E68" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="F68" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>61</v>
       </c>
       <c r="B69" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C69" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="D69" s="2">
-        <v>43512.02811368056</v>
-      </c>
-      <c r="E69" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
+        <v>43512.028113680557</v>
+      </c>
+      <c r="F69" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>62</v>
       </c>
       <c r="B70" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C70" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="D70" s="2">
-        <v>43514.58475023148</v>
-      </c>
-      <c r="E70" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
+        <v>43514.584750231479</v>
+      </c>
+      <c r="F70" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>63</v>
       </c>
       <c r="B71" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C71" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="D71" s="2">
-        <v>43514.58475289352</v>
-      </c>
-      <c r="E71" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
+        <v>43514.584752893519</v>
+      </c>
+      <c r="F71" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>64</v>
       </c>
       <c r="B72" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C72" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="D72" s="2">
-        <v>43514.58475601852</v>
-      </c>
-      <c r="E72" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
+        <v>43514.584756018521</v>
+      </c>
+      <c r="F72" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>65</v>
       </c>
       <c r="B73" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C73" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="D73" s="2">
-        <v>43514.58475809028</v>
-      </c>
-      <c r="E73" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
+        <v>43514.584758090277</v>
+      </c>
+      <c r="F73" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>66</v>
       </c>
       <c r="B74" t="s">
+        <v>81</v>
+      </c>
+      <c r="C74" t="s">
+        <v>167</v>
+      </c>
+      <c r="D74" s="2">
+        <v>43515.482389502307</v>
+      </c>
+      <c r="F74" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>67</v>
+      </c>
+      <c r="B75" t="s">
+        <v>82</v>
+      </c>
+      <c r="C75" t="s">
+        <v>168</v>
+      </c>
+      <c r="D75" s="2">
+        <v>43515.73058116898</v>
+      </c>
+      <c r="F75" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>68</v>
+      </c>
+      <c r="B76" t="s">
+        <v>83</v>
+      </c>
+      <c r="C76" t="s">
+        <v>169</v>
+      </c>
+      <c r="D76" s="2">
+        <v>43515.730583240736</v>
+      </c>
+      <c r="F76" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>69</v>
+      </c>
+      <c r="B77" t="s">
+        <v>84</v>
+      </c>
+      <c r="C77" t="s">
+        <v>170</v>
+      </c>
+      <c r="D77" s="2">
+        <v>43516.495305937497</v>
+      </c>
+      <c r="F77" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>70</v>
+      </c>
+      <c r="B78" t="s">
+        <v>85</v>
+      </c>
+      <c r="C78" t="s">
+        <v>171</v>
+      </c>
+      <c r="D78" s="2">
+        <v>43518.612598460648</v>
+      </c>
+      <c r="F78" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>71</v>
+      </c>
+      <c r="B79" t="s">
+        <v>86</v>
+      </c>
+      <c r="C79" t="s">
+        <v>172</v>
+      </c>
+      <c r="D79" s="2">
+        <v>43521.621568703697</v>
+      </c>
+      <c r="F79" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>72</v>
+      </c>
+      <c r="B80" t="s">
+        <v>87</v>
+      </c>
+      <c r="C80" t="s">
+        <v>173</v>
+      </c>
+      <c r="D80" s="2">
+        <v>43521.621570266201</v>
+      </c>
+      <c r="F80" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>73</v>
+      </c>
+      <c r="B81" t="s">
+        <v>88</v>
+      </c>
+      <c r="C81" t="s">
+        <v>174</v>
+      </c>
+      <c r="D81" s="2">
+        <v>43521.621574733799</v>
+      </c>
+      <c r="F81" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>74</v>
+      </c>
+      <c r="B82" t="s">
+        <v>89</v>
+      </c>
+      <c r="C82" t="s">
+        <v>175</v>
+      </c>
+      <c r="D82" s="2">
+        <v>43521.621574733799</v>
+      </c>
+      <c r="F82" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>75</v>
+      </c>
+      <c r="B83" t="s">
+        <v>90</v>
+      </c>
+      <c r="C83" t="s">
+        <v>176</v>
+      </c>
+      <c r="D83" s="2">
+        <v>43522.716105196763</v>
+      </c>
+      <c r="F83" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>76</v>
+      </c>
+      <c r="B84" t="s">
+        <v>91</v>
+      </c>
+      <c r="C84" t="s">
+        <v>177</v>
+      </c>
+      <c r="D84" s="2">
+        <v>43522.716108946763</v>
+      </c>
+      <c r="F84" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>77</v>
+      </c>
+      <c r="B85" t="s">
+        <v>92</v>
+      </c>
+      <c r="C85" t="s">
+        <v>178</v>
+      </c>
+      <c r="D85" s="2">
+        <v>43523.389754560187</v>
+      </c>
+      <c r="F85" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>78</v>
+      </c>
+      <c r="B86" t="s">
+        <v>93</v>
+      </c>
+      <c r="C86" t="s">
+        <v>179</v>
+      </c>
+      <c r="D86" s="2">
+        <v>43524.459396909719</v>
+      </c>
+      <c r="F86" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>79</v>
+      </c>
+      <c r="B87" t="s">
+        <v>94</v>
+      </c>
+      <c r="C87" t="s">
+        <v>180</v>
+      </c>
+      <c r="D87" s="2">
+        <v>43524.459918932538</v>
+      </c>
+      <c r="F87" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88">
         <v>80</v>
       </c>
-      <c r="C74" t="s">
-        <v>153</v>
-      </c>
-      <c r="D74" s="2">
-        <v>43515.48238950485</v>
-      </c>
-      <c r="E74" t="s">
-        <v>155</v>
+      <c r="B88" t="s">
+        <v>191</v>
+      </c>
+      <c r="C88" t="s">
+        <v>190</v>
+      </c>
+      <c r="D88" s="2">
+        <v>43524.459918932538</v>
+      </c>
+      <c r="F88" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>81</v>
+      </c>
+      <c r="B89" t="s">
+        <v>193</v>
+      </c>
+      <c r="C89" t="s">
+        <v>192</v>
+      </c>
+      <c r="D89" s="2">
+        <v>43524.459918932538</v>
+      </c>
+      <c r="F89" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add write to txt functionality
</commit_message>
<xml_diff>
--- a/New Products Assmt.xlsx
+++ b/New Products Assmt.xlsx
@@ -1,29 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wahyu\PT Telekomunikasi Selular\muhammad_f_rais - POSTPAID REVAS onedrive\New Products Assurance\2019-02\email\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="114_{A497BF04-5BFF-4F7D-8CF1-BD4341CAC932}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{046F0ED7-98A8-446E-8BCF-E462351BC267}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -315,6 +301,12 @@
     <t>017/SV.05/CM-61/II/2019</t>
   </si>
   <si>
+    <t>0214/MK.05/PS-05/II/2019</t>
+  </si>
+  <si>
+    <t>048/MK.05/MK-01/II/2019</t>
+  </si>
+  <si>
     <t>[Nota Dinas] Permohonan Batch Offer untuk Pelanggan BC 06 per Januari 2019 (005/MK.05/PS-03/I/2019)</t>
   </si>
   <si>
@@ -573,6 +565,12 @@
     <t>FW: [Nota Dinas] Permohonan Migration APN Corporate Legacy KEMENKEU Menjadi M2M (017/SV.05/CM-61/II/2019)</t>
   </si>
   <si>
+    <t>[Nota Dinas] Status Kesiapan Komersial (RFC) Paket Promo Roaming Eropa dan Amerika di B2B2C (1 dan 30 Hari Internet &amp;amp;3in1).pdf</t>
+  </si>
+  <si>
+    <t>48 - Sosialisasi Program Quick Win Family Plan</t>
+  </si>
+  <si>
     <t>in progress</t>
   </si>
   <si>
@@ -598,28 +596,16 @@
   </si>
   <si>
     <t>Konfirmasi perubahan behaviour paket roaming, dimana sebelumnya bersifat akumulatif menjadi terpisah per paket. Mekanisme charging sama persis dg sebelum perubahan. Tiap customer disediakan bucket packet 5 sd 15 bucket.</t>
-  </si>
-  <si>
-    <t>[Nota Dinas] Status Kesiapan Komersial (RFC) Paket Promo Roaming Eropa dan Amerika di B2B2C (1 dan 30 Hari Internet &amp;amp;3in1).pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0214/MK.05/PS-05/II/2019 </t>
-  </si>
-  <si>
-    <t>48 - Sosialisasi Program Quick Win Family Plan</t>
-  </si>
-  <si>
-    <t>048/MK.05/MK-01/II/2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -683,14 +669,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -737,7 +715,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -769,27 +747,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -821,24 +781,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1014,19 +956,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1055,7 +992,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1063,22 +1000,22 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2">
         <v>43480</v>
       </c>
       <c r="F2" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="G2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="I2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1086,22 +1023,22 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D3" s="2">
         <v>43480</v>
       </c>
       <c r="F3" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="G3" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="I3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1109,16 +1046,16 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D4" s="2">
         <v>43481</v>
       </c>
       <c r="F4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1126,16 +1063,16 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D5" s="2">
         <v>43481</v>
       </c>
       <c r="F5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>0</v>
       </c>
@@ -1143,19 +1080,19 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D6" s="2">
         <v>43483</v>
       </c>
       <c r="F6" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="I6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1163,19 +1100,19 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D7" s="2">
         <v>43487</v>
       </c>
       <c r="F7" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="G7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1183,16 +1120,16 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D8" s="2">
         <v>43493</v>
       </c>
       <c r="F8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1200,16 +1137,16 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D9" s="2">
         <v>43510</v>
       </c>
       <c r="F9" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1217,16 +1154,16 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D10" s="2">
         <v>43510</v>
       </c>
       <c r="F10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1234,16 +1171,16 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D11" s="2">
         <v>43510</v>
       </c>
       <c r="F11" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1251,16 +1188,16 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D12" s="2">
         <v>43510</v>
       </c>
       <c r="F12" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1268,16 +1205,16 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D13" s="2">
         <v>43510</v>
       </c>
       <c r="F13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1285,16 +1222,16 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D14" s="2">
         <v>43510</v>
       </c>
       <c r="F14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1302,16 +1239,16 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D15" s="2">
         <v>43510</v>
       </c>
       <c r="F15" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1319,16 +1256,16 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D16" s="2">
         <v>43510</v>
       </c>
       <c r="F16" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>9</v>
       </c>
@@ -1336,16 +1273,16 @@
         <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D17" s="2">
         <v>43510</v>
       </c>
       <c r="F17" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>10</v>
       </c>
@@ -1353,16 +1290,16 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D18" s="2">
         <v>43510</v>
       </c>
       <c r="F18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>11</v>
       </c>
@@ -1370,16 +1307,16 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D19" s="2">
         <v>43510</v>
       </c>
       <c r="F19" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>12</v>
       </c>
@@ -1387,16 +1324,16 @@
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D20" s="2">
         <v>43510</v>
       </c>
       <c r="F20" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>13</v>
       </c>
@@ -1404,16 +1341,16 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D21" s="2">
         <v>43510</v>
       </c>
       <c r="F21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>14</v>
       </c>
@@ -1421,16 +1358,16 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D22" s="2">
         <v>43510</v>
       </c>
       <c r="F22" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>15</v>
       </c>
@@ -1438,16 +1375,16 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D23" s="2">
         <v>43510</v>
       </c>
       <c r="F23" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>16</v>
       </c>
@@ -1455,16 +1392,16 @@
         <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D24" s="2">
         <v>43510</v>
       </c>
       <c r="F24" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>17</v>
       </c>
@@ -1472,16 +1409,16 @@
         <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D25" s="2">
         <v>43510</v>
       </c>
       <c r="F25" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>18</v>
       </c>
@@ -1489,16 +1426,16 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D26" s="2">
         <v>43510</v>
       </c>
       <c r="F26" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>19</v>
       </c>
@@ -1506,16 +1443,16 @@
         <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D27" s="2">
         <v>43510</v>
       </c>
       <c r="F27" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>20</v>
       </c>
@@ -1523,16 +1460,16 @@
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D28" s="2">
         <v>43510</v>
       </c>
       <c r="F28" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>21</v>
       </c>
@@ -1540,16 +1477,16 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D29" s="2">
         <v>43510</v>
       </c>
       <c r="F29" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>22</v>
       </c>
@@ -1557,16 +1494,16 @@
         <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D30" s="2">
         <v>43510</v>
       </c>
       <c r="F30" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>23</v>
       </c>
@@ -1574,16 +1511,16 @@
         <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D31" s="2">
         <v>43510</v>
       </c>
       <c r="F31" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>24</v>
       </c>
@@ -1591,16 +1528,16 @@
         <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D32" s="2">
         <v>43510</v>
       </c>
       <c r="F32" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>25</v>
       </c>
@@ -1608,16 +1545,16 @@
         <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D33" s="2">
         <v>43510</v>
       </c>
       <c r="F33" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>26</v>
       </c>
@@ -1625,16 +1562,16 @@
         <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D34" s="2">
         <v>43510</v>
       </c>
       <c r="F34" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>27</v>
       </c>
@@ -1642,16 +1579,16 @@
         <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D35" s="2">
         <v>43510</v>
       </c>
       <c r="F35" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>28</v>
       </c>
@@ -1659,16 +1596,16 @@
         <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D36" s="2">
         <v>43510</v>
       </c>
       <c r="F36" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>29</v>
       </c>
@@ -1676,16 +1613,16 @@
         <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D37" s="2">
         <v>43510</v>
       </c>
       <c r="F37" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>30</v>
       </c>
@@ -1693,16 +1630,16 @@
         <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D38" s="2">
         <v>43511</v>
       </c>
       <c r="F38" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>31</v>
       </c>
@@ -1710,16 +1647,16 @@
         <v>46</v>
       </c>
       <c r="C39" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D39" s="2">
         <v>43511</v>
       </c>
       <c r="F39" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>32</v>
       </c>
@@ -1727,16 +1664,16 @@
         <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D40" s="2">
         <v>43511</v>
       </c>
       <c r="F40" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>33</v>
       </c>
@@ -1744,22 +1681,22 @@
         <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D41" s="2">
         <v>43511</v>
       </c>
       <c r="F41" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="G41" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="I41" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>34</v>
       </c>
@@ -1767,16 +1704,16 @@
         <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D42" s="2">
         <v>43511</v>
       </c>
       <c r="F42" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>35</v>
       </c>
@@ -1784,16 +1721,16 @@
         <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D43" s="2">
         <v>43511</v>
       </c>
       <c r="F43" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>36</v>
       </c>
@@ -1801,16 +1738,16 @@
         <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D44" s="2">
         <v>43511</v>
       </c>
       <c r="F44" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>37</v>
       </c>
@@ -1818,16 +1755,16 @@
         <v>52</v>
       </c>
       <c r="C45" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D45" s="2">
         <v>43511</v>
       </c>
       <c r="F45" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>38</v>
       </c>
@@ -1835,16 +1772,16 @@
         <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D46" s="2">
         <v>43511</v>
       </c>
       <c r="F46" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47">
         <v>39</v>
       </c>
@@ -1852,16 +1789,16 @@
         <v>54</v>
       </c>
       <c r="C47" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D47" s="2">
         <v>43511</v>
       </c>
       <c r="F47" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48">
         <v>40</v>
       </c>
@@ -1869,16 +1806,16 @@
         <v>55</v>
       </c>
       <c r="C48" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D48" s="2">
         <v>43511</v>
       </c>
       <c r="F48" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>41</v>
       </c>
@@ -1886,16 +1823,16 @@
         <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D49" s="2">
         <v>43511</v>
       </c>
       <c r="F49" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>42</v>
       </c>
@@ -1903,16 +1840,16 @@
         <v>57</v>
       </c>
       <c r="C50" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D50" s="2">
         <v>43511</v>
       </c>
       <c r="F50" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51">
         <v>43</v>
       </c>
@@ -1920,16 +1857,16 @@
         <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D51" s="2">
         <v>43511</v>
       </c>
       <c r="F51" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52">
         <v>44</v>
       </c>
@@ -1937,16 +1874,16 @@
         <v>59</v>
       </c>
       <c r="C52" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D52" s="2">
         <v>43511</v>
       </c>
       <c r="F52" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53">
         <v>45</v>
       </c>
@@ -1954,16 +1891,16 @@
         <v>60</v>
       </c>
       <c r="C53" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D53" s="2">
         <v>43511</v>
       </c>
       <c r="F53" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54">
         <v>46</v>
       </c>
@@ -1971,16 +1908,16 @@
         <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D54" s="2">
         <v>43511</v>
       </c>
       <c r="F54" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55">
         <v>47</v>
       </c>
@@ -1988,16 +1925,16 @@
         <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D55" s="2">
         <v>43511</v>
       </c>
       <c r="F55" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56">
         <v>48</v>
       </c>
@@ -2005,16 +1942,16 @@
         <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D56" s="2">
         <v>43511</v>
       </c>
       <c r="F56" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57">
         <v>49</v>
       </c>
@@ -2022,16 +1959,16 @@
         <v>64</v>
       </c>
       <c r="C57" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D57" s="2">
         <v>43511</v>
       </c>
       <c r="F57" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58">
         <v>50</v>
       </c>
@@ -2039,16 +1976,16 @@
         <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D58" s="2">
         <v>43511</v>
       </c>
       <c r="F58" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59">
         <v>51</v>
       </c>
@@ -2056,16 +1993,16 @@
         <v>66</v>
       </c>
       <c r="C59" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D59" s="2">
         <v>43511</v>
       </c>
       <c r="F59" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60">
         <v>52</v>
       </c>
@@ -2073,16 +2010,16 @@
         <v>67</v>
       </c>
       <c r="C60" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D60" s="2">
         <v>43511</v>
       </c>
       <c r="F60" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61">
         <v>53</v>
       </c>
@@ -2090,16 +2027,16 @@
         <v>68</v>
       </c>
       <c r="C61" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D61" s="2">
         <v>43511</v>
       </c>
       <c r="F61" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62">
         <v>54</v>
       </c>
@@ -2107,16 +2044,16 @@
         <v>69</v>
       </c>
       <c r="C62" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D62" s="2">
         <v>43511</v>
       </c>
       <c r="F62" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63">
         <v>55</v>
       </c>
@@ -2124,16 +2061,16 @@
         <v>70</v>
       </c>
       <c r="C63" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D63" s="2">
         <v>43511</v>
       </c>
       <c r="F63" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64">
         <v>56</v>
       </c>
@@ -2141,16 +2078,16 @@
         <v>71</v>
       </c>
       <c r="C64" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D64" s="2">
         <v>43511</v>
       </c>
       <c r="F64" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65">
         <v>57</v>
       </c>
@@ -2158,16 +2095,16 @@
         <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D65" s="2">
         <v>43511</v>
       </c>
       <c r="F65" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66">
         <v>58</v>
       </c>
@@ -2175,16 +2112,16 @@
         <v>73</v>
       </c>
       <c r="C66" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D66" s="2">
         <v>43511</v>
       </c>
       <c r="F66" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67">
         <v>59</v>
       </c>
@@ -2192,16 +2129,16 @@
         <v>74</v>
       </c>
       <c r="C67" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D67" s="2">
         <v>43511</v>
       </c>
       <c r="F67" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68">
         <v>60</v>
       </c>
@@ -2209,16 +2146,16 @@
         <v>75</v>
       </c>
       <c r="C68" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D68" s="2">
         <v>43511</v>
       </c>
       <c r="F68" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69">
         <v>61</v>
       </c>
@@ -2226,16 +2163,16 @@
         <v>76</v>
       </c>
       <c r="C69" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D69" s="2">
-        <v>43512.028113680557</v>
+        <v>43512.02811368056</v>
       </c>
       <c r="F69" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70">
         <v>62</v>
       </c>
@@ -2243,16 +2180,16 @@
         <v>77</v>
       </c>
       <c r="C70" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D70" s="2">
-        <v>43514.584750231479</v>
+        <v>43514.58475023148</v>
       </c>
       <c r="F70" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71">
         <v>63</v>
       </c>
@@ -2260,16 +2197,16 @@
         <v>78</v>
       </c>
       <c r="C71" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D71" s="2">
-        <v>43514.584752893519</v>
+        <v>43514.58475289352</v>
       </c>
       <c r="F71" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72">
         <v>64</v>
       </c>
@@ -2277,16 +2214,16 @@
         <v>79</v>
       </c>
       <c r="C72" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D72" s="2">
-        <v>43514.584756018521</v>
+        <v>43514.58475601852</v>
       </c>
       <c r="F72" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73">
         <v>65</v>
       </c>
@@ -2294,16 +2231,16 @@
         <v>80</v>
       </c>
       <c r="C73" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D73" s="2">
-        <v>43514.584758090277</v>
+        <v>43514.58475809028</v>
       </c>
       <c r="F73" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74">
         <v>66</v>
       </c>
@@ -2311,16 +2248,16 @@
         <v>81</v>
       </c>
       <c r="C74" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D74" s="2">
-        <v>43515.482389502307</v>
+        <v>43515.48238950231</v>
       </c>
       <c r="F74" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75">
         <v>67</v>
       </c>
@@ -2328,16 +2265,16 @@
         <v>82</v>
       </c>
       <c r="C75" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D75" s="2">
         <v>43515.73058116898</v>
       </c>
       <c r="F75" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76">
         <v>68</v>
       </c>
@@ -2345,16 +2282,16 @@
         <v>83</v>
       </c>
       <c r="C76" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D76" s="2">
-        <v>43515.730583240736</v>
+        <v>43515.73058324074</v>
       </c>
       <c r="F76" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77">
         <v>69</v>
       </c>
@@ -2362,16 +2299,16 @@
         <v>84</v>
       </c>
       <c r="C77" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D77" s="2">
-        <v>43516.495305937497</v>
+        <v>43516.4953059375</v>
       </c>
       <c r="F77" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78">
         <v>70</v>
       </c>
@@ -2379,16 +2316,16 @@
         <v>85</v>
       </c>
       <c r="C78" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D78" s="2">
-        <v>43518.612598460648</v>
+        <v>43518.61259846065</v>
       </c>
       <c r="F78" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79">
         <v>71</v>
       </c>
@@ -2396,16 +2333,16 @@
         <v>86</v>
       </c>
       <c r="C79" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D79" s="2">
-        <v>43521.621568703697</v>
+        <v>43521.6215687037</v>
       </c>
       <c r="F79" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80">
         <v>72</v>
       </c>
@@ -2413,16 +2350,16 @@
         <v>87</v>
       </c>
       <c r="C80" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D80" s="2">
-        <v>43521.621570266201</v>
+        <v>43521.6215702662</v>
       </c>
       <c r="F80" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81">
         <v>73</v>
       </c>
@@ -2430,16 +2367,16 @@
         <v>88</v>
       </c>
       <c r="C81" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D81" s="2">
-        <v>43521.621574733799</v>
+        <v>43521.6215747338</v>
       </c>
       <c r="F81" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82">
         <v>74</v>
       </c>
@@ -2447,16 +2384,16 @@
         <v>89</v>
       </c>
       <c r="C82" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D82" s="2">
-        <v>43521.621574733799</v>
+        <v>43521.6215747338</v>
       </c>
       <c r="F82" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83">
         <v>75</v>
       </c>
@@ -2464,16 +2401,16 @@
         <v>90</v>
       </c>
       <c r="C83" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D83" s="2">
-        <v>43522.716105196763</v>
+        <v>43522.71610519676</v>
       </c>
       <c r="F83" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84">
         <v>76</v>
       </c>
@@ -2481,16 +2418,16 @@
         <v>91</v>
       </c>
       <c r="C84" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D84" s="2">
-        <v>43522.716108946763</v>
+        <v>43522.71610894676</v>
       </c>
       <c r="F84" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85">
         <v>77</v>
       </c>
@@ -2498,16 +2435,16 @@
         <v>92</v>
       </c>
       <c r="C85" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D85" s="2">
-        <v>43523.389754560187</v>
+        <v>43523.38975456019</v>
       </c>
       <c r="F85" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86">
         <v>78</v>
       </c>
@@ -2515,16 +2452,16 @@
         <v>93</v>
       </c>
       <c r="C86" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D86" s="2">
-        <v>43524.459396909719</v>
+        <v>43524.45939690972</v>
       </c>
       <c r="F86" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87">
         <v>79</v>
       </c>
@@ -2532,47 +2469,47 @@
         <v>94</v>
       </c>
       <c r="C87" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D87" s="2">
-        <v>43524.459918932538</v>
+        <v>43524.45991893519</v>
       </c>
       <c r="F87" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88">
         <v>80</v>
       </c>
       <c r="B88" t="s">
-        <v>191</v>
+        <v>95</v>
       </c>
       <c r="C88" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D88" s="2">
-        <v>43524.459918932538</v>
+        <v>43524.45991893519</v>
       </c>
       <c r="F88" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89">
         <v>81</v>
       </c>
       <c r="B89" t="s">
-        <v>193</v>
+        <v>96</v>
       </c>
       <c r="C89" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D89" s="2">
-        <v>43524.459918932538</v>
+        <v>43524.45991893519</v>
       </c>
       <c r="F89" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Truncate eml file if its too long
</commit_message>
<xml_diff>
--- a/New Products Assmt.xlsx
+++ b/New Products Assmt.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="309">
   <si>
     <t>No</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Remark</t>
   </si>
   <si>
+    <t>Folder</t>
+  </si>
+  <si>
     <t>005/MK.05/PS-03/I/2019</t>
   </si>
   <si>
@@ -307,6 +310,36 @@
     <t>048/MK.05/MK-01/II/2019</t>
   </si>
   <si>
+    <t>045/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>0225/MK.05/PS-05/III/2019</t>
+  </si>
+  <si>
+    <t>028/MK.05/PS-37/III/2019</t>
+  </si>
+  <si>
+    <t>0224/MK.05/PS-05/III/2019</t>
+  </si>
+  <si>
+    <t>046/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>050/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>024/IS.01/IY-04/III/2019</t>
+  </si>
+  <si>
+    <t>052/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>049/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>0234/MK.05/PS-05/III/2019</t>
+  </si>
+  <si>
     <t>[Nota Dinas] Permohonan Batch Offer untuk Pelanggan BC 06 per Januari 2019 (005/MK.05/PS-03/I/2019)</t>
   </si>
   <si>
@@ -571,6 +604,36 @@
     <t>48 - Sosialisasi Program Quick Win Family Plan</t>
   </si>
   <si>
+    <t>FW: [Nota Dinas] Pemberitahuan RFI Extend Coverage Roaming (OCSke5th2019) (045/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>FW: [Nota Dinas] Status Kesiapan Komersial (RFC) Halo Kick Bundling Samsung S10 (0225/MK.05/PS-05/III/2019)</t>
+  </si>
+  <si>
+    <t>FW: [Nota Dinas] Pemberitahuan Revisi RFS Halo Kick Bundling Samsung S10 (028/MK.05/PS-37/III/2019)</t>
+  </si>
+  <si>
+    <t>FW: [Nota Dinas] Status Kesiapan Komersial (RFC) Fitur PSB TDW (0224/MK.05/PS-05/III/2019)</t>
+  </si>
+  <si>
+    <t>FW: [Nota Dinas] Pemberitahuan RFI Migration Roaming Prepaid Non-Rollover Ph1 (046/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>FW: [Nota Dinas] Pemberitahuan RFS Paket Roaming Prepaid Standalone API Digicore pada UMB (Umroh dan Promo Asia Australia) (050/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>Fwd: [Nota Dinas] Permohonan Migrasi APN Corporate Individual (024/IS.01/IY-04/III/2019)</t>
+  </si>
+  <si>
+    <t>FW: [Nota Dinas] Pemberitahuan RFS Paket Halo Kick HVC Bank 300K (OMSKe1Th2019) (052/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>FW: [Nota Dinas] Pemberitahuan RFS Paket Roaming Prepaid Standalone API Digicore pada UMB (Promo Eropa Amerika, Asia Reguler, Eropa Reguler, Amerika Afrika, dan Haji) (049/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>FW: [Nota Dinas] Status Kesiapan Komersial (RFC) Produk Premium Bundling MD Pictures (Postpaid) (0234/MK.05/PS-05/III/2019)</t>
+  </si>
+  <si>
     <t>in progress</t>
   </si>
   <si>
@@ -596,6 +659,288 @@
   </si>
   <si>
     <t>Konfirmasi perubahan behaviour paket roaming, dimana sebelumnya bersifat akumulatif menjadi terpisah per paket. Mekanisme charging sama persis dg sebelum perubahan. Tiap customer disediakan bucket packet 5 sd 15 bucket.</t>
+  </si>
+  <si>
+    <t>005MK.05PS-03I2019</t>
+  </si>
+  <si>
+    <t>020MK.05PS-05I2019</t>
+  </si>
+  <si>
+    <t>028MK.05PS-05I2019</t>
+  </si>
+  <si>
+    <t>0334IS.01EN-01I2019</t>
+  </si>
+  <si>
+    <t>011MK.05PS-33I2019</t>
+  </si>
+  <si>
+    <t>006MK.05PS-37I2019</t>
+  </si>
+  <si>
+    <t>OMS 010MK.05PS-37I2019</t>
+  </si>
+  <si>
+    <t>018MK.05PS-37II2019</t>
+  </si>
+  <si>
+    <t>UMB 0113MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>023MK.05PS-33II2019</t>
+  </si>
+  <si>
+    <t>021MK.05PS-33II2019</t>
+  </si>
+  <si>
+    <t>025MK.05PS-33II2019</t>
+  </si>
+  <si>
+    <t>0132MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>021MK.05PS-37II2019</t>
+  </si>
+  <si>
+    <t>0136MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>0137MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>0102MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>019MK.05PS-33II2019</t>
+  </si>
+  <si>
+    <t>014MK.05PS-37II2019</t>
+  </si>
+  <si>
+    <t>013MK.05PS-37II2019</t>
+  </si>
+  <si>
+    <t>016MK.05PS-37II2019</t>
+  </si>
+  <si>
+    <t>015MK.05PS-37II2019</t>
+  </si>
+  <si>
+    <t>0110MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>017MK.05PS-37II2019</t>
+  </si>
+  <si>
+    <t>019MK.05PS-37II2019</t>
+  </si>
+  <si>
+    <t>0118MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>023MK.05PS-03II2019</t>
+  </si>
+  <si>
+    <t>024MK.05PS-03II2019</t>
+  </si>
+  <si>
+    <t>020MK.05PS-37II2019</t>
+  </si>
+  <si>
+    <t>093MK.05PS-05I2019</t>
+  </si>
+  <si>
+    <t>090MK.05PS-05I2019</t>
+  </si>
+  <si>
+    <t>088MK.05PS-05I2019</t>
+  </si>
+  <si>
+    <t>089MK.05PS-05I2019</t>
+  </si>
+  <si>
+    <t>017MK.05PS-03I2019</t>
+  </si>
+  <si>
+    <t>015MK.05PS-33I2019</t>
+  </si>
+  <si>
+    <t>077MK.05PS-05I2019</t>
+  </si>
+  <si>
+    <t>073MK.05PS-05I2019</t>
+  </si>
+  <si>
+    <t>01438MK.05PS-05I2019</t>
+  </si>
+  <si>
+    <t>023MK.05PS-37II2019</t>
+  </si>
+  <si>
+    <t>030MK.05PS-33II2019</t>
+  </si>
+  <si>
+    <t>0155MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>0158MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>064MK.05PS-05I2019</t>
+  </si>
+  <si>
+    <t>003MK.05PS-05I2019</t>
+  </si>
+  <si>
+    <t>065MK.05PS-05I2019</t>
+  </si>
+  <si>
+    <t>052MK.05PS-05I2019</t>
+  </si>
+  <si>
+    <t>048MK.05PS-05I2019</t>
+  </si>
+  <si>
+    <t>047MK.05PS-05I2019</t>
+  </si>
+  <si>
+    <t>004SV.05CM-61I2019</t>
+  </si>
+  <si>
+    <t>008SV.05CM-61I2019</t>
+  </si>
+  <si>
+    <t>005SV.05CM-61I2019</t>
+  </si>
+  <si>
+    <t>008MK.05PS-03I2019</t>
+  </si>
+  <si>
+    <t>001MK.05PS-03I2019</t>
+  </si>
+  <si>
+    <t>009MK.05PS-33I2019</t>
+  </si>
+  <si>
+    <t>003MK.05PS-37I2019</t>
+  </si>
+  <si>
+    <t>010MK.05PS-33I2019</t>
+  </si>
+  <si>
+    <t>012MK.05PS-33I2019</t>
+  </si>
+  <si>
+    <t>009MK.05PS-37I2019</t>
+  </si>
+  <si>
+    <t>005MK.05PS-37I2019</t>
+  </si>
+  <si>
+    <t>007MK.05PS-33I2019</t>
+  </si>
+  <si>
+    <t>006MK.05PS-33I2019</t>
+  </si>
+  <si>
+    <t>001MK.05PS-33I2019</t>
+  </si>
+  <si>
+    <t>014MK.05PS-33I2019</t>
+  </si>
+  <si>
+    <t>013MK.05PS-33I2019</t>
+  </si>
+  <si>
+    <t>008MK.05PS-33I2019</t>
+  </si>
+  <si>
+    <t>007MK.05PS-37I2019</t>
+  </si>
+  <si>
+    <t>008MK.05PS-37I2019</t>
+  </si>
+  <si>
+    <t>031MK.05PS-33II2019</t>
+  </si>
+  <si>
+    <t>0169MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>0170MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>0171MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>028MK.05PS-03II2019</t>
+  </si>
+  <si>
+    <t>033MK.05PS-33II2019</t>
+  </si>
+  <si>
+    <t>029MK.05PS-03II2019</t>
+  </si>
+  <si>
+    <t>037MK.05PS-33II2019</t>
+  </si>
+  <si>
+    <t>0192MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>032MK.05PS-03II2019</t>
+  </si>
+  <si>
+    <t>031MK.05PS-03II2019</t>
+  </si>
+  <si>
+    <t>0197MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>042MK.05PS-33II2019</t>
+  </si>
+  <si>
+    <t>034MK.05PS-03II2019</t>
+  </si>
+  <si>
+    <t>0208MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>027MK.05PS-37II2019</t>
+  </si>
+  <si>
+    <t>016SV.05CM-61II2019</t>
+  </si>
+  <si>
+    <t>017SV.05CM-61II2019</t>
+  </si>
+  <si>
+    <t>0214MK.05PS-05II2019</t>
+  </si>
+  <si>
+    <t>048MK.05MK-01II2019</t>
+  </si>
+  <si>
+    <t>045MK.05PS-33III2019</t>
+  </si>
+  <si>
+    <t>0225MK.05PS-05III2019</t>
+  </si>
+  <si>
+    <t>028MK.05PS-37III2019</t>
+  </si>
+  <si>
+    <t>0224MK.05PS-05III2019</t>
+  </si>
+  <si>
+    <t>046MK.05PS-33III2019</t>
+  </si>
+  <si>
+    <t>050MK.05PS-33III2019</t>
+  </si>
+  <si>
+    <t>024IS.01IY-04III2019</t>
   </si>
 </sst>
 </file>
@@ -957,13 +1302,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -991,1525 +1336,1983 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="D2" s="2">
         <v>43480</v>
       </c>
       <c r="F2" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="G2" t="s">
-        <v>187</v>
+        <v>208</v>
       </c>
       <c r="I2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>211</v>
+      </c>
+      <c r="J2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="D3" s="2">
         <v>43480</v>
       </c>
       <c r="F3" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="G3" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="I3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>212</v>
+      </c>
+      <c r="J3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="D4" s="2">
         <v>43481</v>
       </c>
       <c r="F4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="D5" s="2">
         <v>43481</v>
       </c>
       <c r="F5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="D6" s="2">
         <v>43483</v>
       </c>
       <c r="F6" t="s">
-        <v>186</v>
+        <v>207</v>
       </c>
       <c r="I6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>213</v>
+      </c>
+      <c r="J6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="D7" s="2">
         <v>43487</v>
       </c>
       <c r="F7" t="s">
-        <v>186</v>
+        <v>207</v>
       </c>
       <c r="G7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>210</v>
+      </c>
+      <c r="J7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="D8" s="2">
         <v>43493</v>
       </c>
       <c r="F8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="D9" s="2">
         <v>43510</v>
       </c>
       <c r="F9" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="D10" s="2">
         <v>43510</v>
       </c>
       <c r="F10" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J10" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="D11" s="2">
         <v>43510</v>
       </c>
       <c r="F11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="D12" s="2">
         <v>43510</v>
       </c>
       <c r="F12" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="D13" s="2">
         <v>43510</v>
       </c>
       <c r="F13" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J13" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="D14" s="2">
         <v>43510</v>
       </c>
       <c r="F14" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J14" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="D15" s="2">
         <v>43510</v>
       </c>
       <c r="F15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J15" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D16" s="2">
         <v>43510</v>
       </c>
       <c r="F16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J16" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D17" s="2">
         <v>43510</v>
       </c>
       <c r="F17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="D18" s="2">
         <v>43510</v>
       </c>
       <c r="F18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J18" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="D19" s="2">
         <v>43510</v>
       </c>
       <c r="F19" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J19" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D20" s="2">
         <v>43510</v>
       </c>
       <c r="F20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J20" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="D21" s="2">
         <v>43510</v>
       </c>
       <c r="F21" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="D22" s="2">
         <v>43510</v>
       </c>
       <c r="F22" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J22" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="D23" s="2">
         <v>43510</v>
       </c>
       <c r="F23" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J23" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="D24" s="2">
         <v>43510</v>
       </c>
       <c r="F24" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J24" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D25" s="2">
         <v>43510</v>
       </c>
       <c r="F25" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J25" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="D26" s="2">
         <v>43510</v>
       </c>
       <c r="F26" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J26" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D27" s="2">
         <v>43510</v>
       </c>
       <c r="F27" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J27" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="D28" s="2">
         <v>43510</v>
       </c>
       <c r="F28" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="D29" s="2">
         <v>43510</v>
       </c>
       <c r="F29" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J29" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="D30" s="2">
         <v>43510</v>
       </c>
       <c r="F30" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J30" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="D31" s="2">
         <v>43510</v>
       </c>
       <c r="F31" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J31" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="D32" s="2">
         <v>43510</v>
       </c>
       <c r="F32" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J32" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="D33" s="2">
         <v>43510</v>
       </c>
       <c r="F33" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J33" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="D34" s="2">
         <v>43510</v>
       </c>
       <c r="F34" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J34" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="D35" s="2">
         <v>43510</v>
       </c>
       <c r="F35" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J35" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="D36" s="2">
         <v>43510</v>
       </c>
       <c r="F36" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J36" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="D37" s="2">
         <v>43510</v>
       </c>
       <c r="F37" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J37" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="D38" s="2">
         <v>43511</v>
       </c>
       <c r="F38" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J38" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="D39" s="2">
         <v>43511</v>
       </c>
       <c r="F39" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J39" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D40" s="2">
         <v>43511</v>
       </c>
       <c r="F40" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J40" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C41" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D41" s="2">
         <v>43511</v>
       </c>
       <c r="F41" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="G41" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="I41" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+        <v>214</v>
+      </c>
+      <c r="J41" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D42" s="2">
         <v>43511</v>
       </c>
       <c r="F42" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="D43" s="2">
         <v>43511</v>
       </c>
       <c r="F43" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J43" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C44" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="D44" s="2">
         <v>43511</v>
       </c>
       <c r="F44" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J44" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="B45" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C45" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D45" s="2">
         <v>43511</v>
       </c>
       <c r="F45" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J45" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C46" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="D46" s="2">
         <v>43511</v>
       </c>
       <c r="F46" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J46" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C47" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="D47" s="2">
         <v>43511</v>
       </c>
       <c r="F47" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+        <v>207</v>
+      </c>
+      <c r="J47" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="D48" s="2">
         <v>43511</v>
       </c>
       <c r="F48" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J48" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="D49" s="2">
         <v>43511</v>
       </c>
       <c r="F49" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J49" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C50" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="D50" s="2">
         <v>43511</v>
       </c>
       <c r="F50" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J50" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="B51" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C51" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="D51" s="2">
         <v>43511</v>
       </c>
       <c r="F51" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J51" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="B52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C52" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="D52" s="2">
         <v>43511</v>
       </c>
       <c r="F52" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J52" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B53" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C53" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="D53" s="2">
         <v>43511</v>
       </c>
       <c r="F53" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J53" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="B54" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C54" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="D54" s="2">
         <v>43511</v>
       </c>
       <c r="F54" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J54" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B55" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C55" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="D55" s="2">
         <v>43511</v>
       </c>
       <c r="F55" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J55" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="B56" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C56" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="D56" s="2">
         <v>43511</v>
       </c>
       <c r="F56" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J56" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C57" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="D57" s="2">
         <v>43511</v>
       </c>
       <c r="F57" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J57" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="B58" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C58" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="D58" s="2">
         <v>43511</v>
       </c>
       <c r="F58" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J58" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="B59" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C59" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="D59" s="2">
         <v>43511</v>
       </c>
       <c r="F59" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J59" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="B60" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C60" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="D60" s="2">
         <v>43511</v>
       </c>
       <c r="F60" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J60" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="B61" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C61" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="D61" s="2">
         <v>43511</v>
       </c>
       <c r="F61" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J61" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C62" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="D62" s="2">
         <v>43511</v>
       </c>
       <c r="F62" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J62" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="B63" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C63" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="D63" s="2">
         <v>43511</v>
       </c>
       <c r="F63" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J63" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C64" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="D64" s="2">
         <v>43511</v>
       </c>
       <c r="F64" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J64" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="B65" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C65" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="D65" s="2">
         <v>43511</v>
       </c>
       <c r="F65" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J65" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="B66" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C66" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="D66" s="2">
         <v>43511</v>
       </c>
       <c r="F66" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J66" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="B67" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C67" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="D67" s="2">
         <v>43511</v>
       </c>
       <c r="F67" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J67" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="B68" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C68" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="D68" s="2">
         <v>43511</v>
       </c>
       <c r="F68" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J68" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="B69" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C69" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="D69" s="2">
         <v>43512.02811368056</v>
       </c>
       <c r="F69" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J69" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="B70" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C70" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="D70" s="2">
         <v>43514.58475023148</v>
       </c>
       <c r="F70" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J70" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C71" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="D71" s="2">
         <v>43514.58475289352</v>
       </c>
       <c r="F71" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J71" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C72" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="D72" s="2">
         <v>43514.58475601852</v>
       </c>
       <c r="F72" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J72" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C73" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="D73" s="2">
         <v>43514.58475809028</v>
       </c>
       <c r="F73" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J73" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="B74" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C74" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="D74" s="2">
         <v>43515.48238950231</v>
       </c>
       <c r="F74" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J74" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C75" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="D75" s="2">
         <v>43515.73058116898</v>
       </c>
       <c r="F75" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J75" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="B76" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C76" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="D76" s="2">
         <v>43515.73058324074</v>
       </c>
       <c r="F76" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J76" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C77" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="D77" s="2">
         <v>43516.4953059375</v>
       </c>
       <c r="F77" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J77" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="B78" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C78" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="D78" s="2">
         <v>43518.61259846065</v>
       </c>
       <c r="F78" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J78" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="B79" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C79" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="D79" s="2">
         <v>43521.6215687037</v>
       </c>
       <c r="F79" t="s">
+        <v>207</v>
+      </c>
+      <c r="J79" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80">
+        <v>0</v>
+      </c>
+      <c r="B80" t="s">
+        <v>88</v>
+      </c>
+      <c r="C80" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80">
-        <v>72</v>
-      </c>
-      <c r="B80" t="s">
-        <v>87</v>
-      </c>
-      <c r="C80" t="s">
-        <v>175</v>
       </c>
       <c r="D80" s="2">
         <v>43521.6215702662</v>
       </c>
       <c r="F80" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J80" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="B81" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C81" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="D81" s="2">
         <v>43521.6215747338</v>
       </c>
       <c r="F81" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J81" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C82" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="D82" s="2">
         <v>43521.6215747338</v>
       </c>
       <c r="F82" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J82" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C83" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="D83" s="2">
         <v>43522.71610519676</v>
       </c>
       <c r="F83" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J83" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="B84" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C84" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="D84" s="2">
         <v>43522.71610894676</v>
       </c>
       <c r="F84" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J84" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="B85" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C85" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="D85" s="2">
         <v>43523.38975456019</v>
       </c>
       <c r="F85" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J85" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="B86" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C86" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="D86" s="2">
         <v>43524.45939690972</v>
       </c>
       <c r="F86" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J86" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="B87" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C87" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="D87" s="2">
         <v>43524.45991893519</v>
       </c>
       <c r="F87" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J87" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="B88" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C88" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="D88" s="2">
         <v>43524.45991893519</v>
       </c>
       <c r="F88" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="J88" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="B89" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C89" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="D89" s="2">
         <v>43524.45991893519</v>
       </c>
       <c r="F89" t="s">
-        <v>186</v>
+        <v>207</v>
+      </c>
+      <c r="J89" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90">
+        <v>1</v>
+      </c>
+      <c r="B90" t="s">
+        <v>98</v>
+      </c>
+      <c r="C90" t="s">
+        <v>196</v>
+      </c>
+      <c r="D90" s="2">
+        <v>43529.37632800926</v>
+      </c>
+      <c r="F90" t="s">
+        <v>207</v>
+      </c>
+      <c r="J90" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91">
+        <v>2</v>
+      </c>
+      <c r="B91" t="s">
+        <v>99</v>
+      </c>
+      <c r="C91" t="s">
+        <v>197</v>
+      </c>
+      <c r="D91" s="2">
+        <v>43529.37633297453</v>
+      </c>
+      <c r="F91" t="s">
+        <v>207</v>
+      </c>
+      <c r="J91" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92">
+        <v>3</v>
+      </c>
+      <c r="B92" t="s">
+        <v>100</v>
+      </c>
+      <c r="C92" t="s">
+        <v>198</v>
+      </c>
+      <c r="D92" s="2">
+        <v>43529.42497050926</v>
+      </c>
+      <c r="F92" t="s">
+        <v>207</v>
+      </c>
+      <c r="J92" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93">
+        <v>4</v>
+      </c>
+      <c r="B93" t="s">
+        <v>101</v>
+      </c>
+      <c r="C93" t="s">
+        <v>199</v>
+      </c>
+      <c r="D93" s="2">
+        <v>43529.42497885416</v>
+      </c>
+      <c r="F93" t="s">
+        <v>207</v>
+      </c>
+      <c r="J93" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94">
+        <v>5</v>
+      </c>
+      <c r="B94" t="s">
+        <v>102</v>
+      </c>
+      <c r="C94" t="s">
+        <v>200</v>
+      </c>
+      <c r="D94" s="2">
+        <v>43529.48534415509</v>
+      </c>
+      <c r="F94" t="s">
+        <v>207</v>
+      </c>
+      <c r="J94" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95">
+        <v>6</v>
+      </c>
+      <c r="B95" t="s">
+        <v>103</v>
+      </c>
+      <c r="C95" t="s">
+        <v>201</v>
+      </c>
+      <c r="D95" s="2">
+        <v>43529.74539105324</v>
+      </c>
+      <c r="F95" t="s">
+        <v>207</v>
+      </c>
+      <c r="J95" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96">
+        <v>7</v>
+      </c>
+      <c r="B96" t="s">
+        <v>104</v>
+      </c>
+      <c r="C96" t="s">
+        <v>202</v>
+      </c>
+      <c r="D96" s="2">
+        <v>43529.75238363426</v>
+      </c>
+      <c r="F96" t="s">
+        <v>207</v>
+      </c>
+      <c r="J96" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97">
+        <v>8</v>
+      </c>
+      <c r="B97" t="s">
+        <v>105</v>
+      </c>
+      <c r="C97" t="s">
+        <v>203</v>
+      </c>
+      <c r="D97" s="2">
+        <v>43529.7523853125</v>
+      </c>
+      <c r="F97" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98">
+        <v>9</v>
+      </c>
+      <c r="B98" t="s">
+        <v>106</v>
+      </c>
+      <c r="C98" t="s">
+        <v>204</v>
+      </c>
+      <c r="D98" s="2">
+        <v>43529.79556278935</v>
+      </c>
+      <c r="F98" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99">
+        <v>10</v>
+      </c>
+      <c r="B99" t="s">
+        <v>107</v>
+      </c>
+      <c r="C99" t="s">
+        <v>205</v>
+      </c>
+      <c r="D99" s="2">
+        <v>43530.39331518118</v>
+      </c>
+      <c r="F99" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add get_attachment_dev.py which download attachment directly from email
</commit_message>
<xml_diff>
--- a/New Products Assmt.xlsx
+++ b/New Products Assmt.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="382">
   <si>
     <t>No</t>
   </si>
@@ -340,6 +340,78 @@
     <t>0234/MK.05/PS-05/III/2019</t>
   </si>
   <si>
+    <t>053/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>0236/MK.05/PS-05/III/2019</t>
+  </si>
+  <si>
+    <t>038/MK.05/PS-03/III/2019</t>
+  </si>
+  <si>
+    <t>054/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>031/MK.05/PS-37/III/2019</t>
+  </si>
+  <si>
+    <t>057/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>056/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>055/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>032/MK.05/PS-37/III/2019</t>
+  </si>
+  <si>
+    <t>0243/MK.05/PS-05/III/2019</t>
+  </si>
+  <si>
+    <t>0246/MK.05/PS-05/III/2019</t>
+  </si>
+  <si>
+    <t>034/MK.05/PS-37/III/2019</t>
+  </si>
+  <si>
+    <t>033/MK.05/PS-37/III/2019</t>
+  </si>
+  <si>
+    <t>0251/MK.05/PS-05/III/2019</t>
+  </si>
+  <si>
+    <t>059/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>060/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>035/MK.05/PS-37/III/2019</t>
+  </si>
+  <si>
+    <t>041/MK.05/PS-03/III/2019</t>
+  </si>
+  <si>
+    <t>0270/MK.05/PS-05/III/2019</t>
+  </si>
+  <si>
+    <t>0269/MK.05/PS-05/III/2019</t>
+  </si>
+  <si>
+    <t>020/SV.05/CM-61/III/2019</t>
+  </si>
+  <si>
+    <t>066/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>0282/MK.05/PS-05/III/2019</t>
+  </si>
+  <si>
+    <t>065/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
     <t>[Nota Dinas] Permohonan Batch Offer untuk Pelanggan BC 06 per Januari 2019 (005/MK.05/PS-03/I/2019)</t>
   </si>
   <si>
@@ -634,6 +706,78 @@
     <t>FW: [Nota Dinas] Status Kesiapan Komersial (RFC) Produk Premium Bundling MD Pictures (Postpaid) (0234/MK.05/PS-05/III/2019)</t>
   </si>
   <si>
+    <t>[Nota Dinas] Pemberitahuan RFS Paket BUMN Sunday Sale (OMSKe4Th2019) (053/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Status Kesiapan Komersial (RFC) Fitur Prepaid2Postpaid TDW (0236/MK.05/PS-05/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Implementasi Roaming Standalone Prepaid (Promo Asia Australia dan Umroh) Ph1 (038/MK.05/PS-03/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFI Paket Roaming Postpaid Standalone pada Sistem Digicore (Umroh, Promo Asia Australia, Promo Eropa Amerika, Asia Reguler, Eropa Reguler, Amerika Afrika, dan Haji) (054/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] PPemberitahuan RFS Surprise Deal Postpaid Maret 2019 (UMB) (031/MK.05/PS-37/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan Revisi RFS Paket BUMN Sunday Sale (OMSKe4Th2019) (057/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan Revisi RFS Paket BUMN Sunday Sale dan Release Digicore (OMSKe4Th2019) (056/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFS Paket BUMN Sunday Sale dan Release Digicore (OMSKe4Th2019) (055/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFS Weekend Deal BUMN 15GB Postpaid Maret 2019 (032/MK.05/PS-37/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Status Kesiapan Komersial (RFC) Paket BUMN Sunday Sale (0243/MK.05/PS-05/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Status Kesiapan Komersial (RFC) Weekend Deal BUMN 15GB Postpaid Maret 2019 (0246/MK.05/PS-05/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFI Surprise Deal Postpaid Maret 2019 (MyTsel) (034/MK.05/PS-37/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFS Surprise Deal Postpaid Maret 2019 (MyTsel) (033/MK.05/PS-37/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Status Kesiapan Komersial (RFC) Surprise Deal Postpaid Maret 2019 (UMB) (0251/MK.05/PS-05/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFI Enhancement CLS Info di My Telkomsel Apps (059/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFI Pemberian Offer Gimmick Setelah Pembayaran Tagihan (060/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFS Paket Family Plan Cross Brand – Postpaid Parent (MyTsel) (035/MK.05/PS-37/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Permohonan Batch Offer untuk Pelanggan BC 06 per Maret 2019 (041/MK.05/PS-03/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Laporan Hasil Inspeksi (ITR) Surprise Deal Postpaid Maret 2019 (MyTsel) (0270/MK.05/PS-05/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Laporan Hasil Inspeksi (ITR) Surprise Deals Prepaid Postpaid 12 Maret 2019 UMB dan Mytsel (0269/MK.05/PS-05/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Permohonan Pembuatan APN Komersial Corporate PLN  UP2D Jakarta (UP2DTSEL) (020/SV.05/CM-61/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFI Perubahan Notifikasi SMS Roaming di Malaysia (066/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Status Kesiapan Komersial (RFC) Paket Family Plan Cross Brand – Postpaid Parent (MyTsel) (0282/MK.05/PS-05/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFI Migration Roaming Prepaid Non-Rollover Ph2 (065/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
     <t>in progress</t>
   </si>
   <si>
@@ -661,286 +805,361 @@
     <t>Konfirmasi perubahan behaviour paket roaming, dimana sebelumnya bersifat akumulatif menjadi terpisah per paket. Mekanisme charging sama persis dg sebelum perubahan. Tiap customer disediakan bucket packet 5 sd 15 bucket.</t>
   </si>
   <si>
-    <t>005MK.05PS-03I2019</t>
-  </si>
-  <si>
-    <t>020MK.05PS-05I2019</t>
-  </si>
-  <si>
-    <t>028MK.05PS-05I2019</t>
-  </si>
-  <si>
-    <t>0334IS.01EN-01I2019</t>
-  </si>
-  <si>
-    <t>011MK.05PS-33I2019</t>
-  </si>
-  <si>
-    <t>006MK.05PS-37I2019</t>
-  </si>
-  <si>
-    <t>OMS 010MK.05PS-37I2019</t>
-  </si>
-  <si>
-    <t>018MK.05PS-37II2019</t>
-  </si>
-  <si>
-    <t>UMB 0113MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>023MK.05PS-33II2019</t>
-  </si>
-  <si>
-    <t>021MK.05PS-33II2019</t>
-  </si>
-  <si>
-    <t>025MK.05PS-33II2019</t>
-  </si>
-  <si>
-    <t>0132MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>021MK.05PS-37II2019</t>
-  </si>
-  <si>
-    <t>0136MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>0137MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>0102MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>019MK.05PS-33II2019</t>
-  </si>
-  <si>
-    <t>014MK.05PS-37II2019</t>
-  </si>
-  <si>
-    <t>013MK.05PS-37II2019</t>
-  </si>
-  <si>
-    <t>016MK.05PS-37II2019</t>
-  </si>
-  <si>
-    <t>015MK.05PS-37II2019</t>
-  </si>
-  <si>
-    <t>0110MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>017MK.05PS-37II2019</t>
-  </si>
-  <si>
-    <t>019MK.05PS-37II2019</t>
-  </si>
-  <si>
-    <t>0118MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>023MK.05PS-03II2019</t>
-  </si>
-  <si>
-    <t>024MK.05PS-03II2019</t>
-  </si>
-  <si>
-    <t>020MK.05PS-37II2019</t>
-  </si>
-  <si>
-    <t>093MK.05PS-05I2019</t>
-  </si>
-  <si>
-    <t>090MK.05PS-05I2019</t>
-  </si>
-  <si>
-    <t>088MK.05PS-05I2019</t>
-  </si>
-  <si>
-    <t>089MK.05PS-05I2019</t>
-  </si>
-  <si>
-    <t>017MK.05PS-03I2019</t>
-  </si>
-  <si>
-    <t>015MK.05PS-33I2019</t>
-  </si>
-  <si>
-    <t>077MK.05PS-05I2019</t>
-  </si>
-  <si>
-    <t>073MK.05PS-05I2019</t>
-  </si>
-  <si>
-    <t>01438MK.05PS-05I2019</t>
-  </si>
-  <si>
-    <t>023MK.05PS-37II2019</t>
-  </si>
-  <si>
-    <t>030MK.05PS-33II2019</t>
-  </si>
-  <si>
-    <t>0155MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>0158MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>064MK.05PS-05I2019</t>
-  </si>
-  <si>
-    <t>003MK.05PS-05I2019</t>
-  </si>
-  <si>
-    <t>065MK.05PS-05I2019</t>
-  </si>
-  <si>
-    <t>052MK.05PS-05I2019</t>
-  </si>
-  <si>
-    <t>048MK.05PS-05I2019</t>
-  </si>
-  <si>
-    <t>047MK.05PS-05I2019</t>
-  </si>
-  <si>
-    <t>004SV.05CM-61I2019</t>
-  </si>
-  <si>
-    <t>008SV.05CM-61I2019</t>
-  </si>
-  <si>
-    <t>005SV.05CM-61I2019</t>
-  </si>
-  <si>
-    <t>008MK.05PS-03I2019</t>
-  </si>
-  <si>
-    <t>001MK.05PS-03I2019</t>
-  </si>
-  <si>
-    <t>009MK.05PS-33I2019</t>
-  </si>
-  <si>
-    <t>003MK.05PS-37I2019</t>
-  </si>
-  <si>
-    <t>010MK.05PS-33I2019</t>
-  </si>
-  <si>
-    <t>012MK.05PS-33I2019</t>
-  </si>
-  <si>
-    <t>009MK.05PS-37I2019</t>
-  </si>
-  <si>
-    <t>005MK.05PS-37I2019</t>
-  </si>
-  <si>
-    <t>007MK.05PS-33I2019</t>
-  </si>
-  <si>
-    <t>006MK.05PS-33I2019</t>
-  </si>
-  <si>
-    <t>001MK.05PS-33I2019</t>
-  </si>
-  <si>
-    <t>014MK.05PS-33I2019</t>
-  </si>
-  <si>
-    <t>013MK.05PS-33I2019</t>
-  </si>
-  <si>
-    <t>008MK.05PS-33I2019</t>
-  </si>
-  <si>
-    <t>007MK.05PS-37I2019</t>
-  </si>
-  <si>
-    <t>008MK.05PS-37I2019</t>
-  </si>
-  <si>
-    <t>031MK.05PS-33II2019</t>
-  </si>
-  <si>
-    <t>0169MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>0170MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>0171MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>028MK.05PS-03II2019</t>
-  </si>
-  <si>
-    <t>033MK.05PS-33II2019</t>
-  </si>
-  <si>
-    <t>029MK.05PS-03II2019</t>
-  </si>
-  <si>
-    <t>037MK.05PS-33II2019</t>
-  </si>
-  <si>
-    <t>0192MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>032MK.05PS-03II2019</t>
-  </si>
-  <si>
-    <t>031MK.05PS-03II2019</t>
-  </si>
-  <si>
-    <t>0197MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>042MK.05PS-33II2019</t>
-  </si>
-  <si>
-    <t>034MK.05PS-03II2019</t>
-  </si>
-  <si>
-    <t>0208MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>027MK.05PS-37II2019</t>
-  </si>
-  <si>
-    <t>016SV.05CM-61II2019</t>
-  </si>
-  <si>
-    <t>017SV.05CM-61II2019</t>
-  </si>
-  <si>
-    <t>0214MK.05PS-05II2019</t>
-  </si>
-  <si>
-    <t>048MK.05MK-01II2019</t>
-  </si>
-  <si>
-    <t>045MK.05PS-33III2019</t>
-  </si>
-  <si>
-    <t>0225MK.05PS-05III2019</t>
-  </si>
-  <si>
-    <t>028MK.05PS-37III2019</t>
-  </si>
-  <si>
-    <t>0224MK.05PS-05III2019</t>
-  </si>
-  <si>
-    <t>046MK.05PS-33III2019</t>
-  </si>
-  <si>
-    <t>050MK.05PS-33III2019</t>
-  </si>
-  <si>
-    <t>024IS.01IY-04III2019</t>
+    <t>005MK05PS-03I2019</t>
+  </si>
+  <si>
+    <t>020MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>028MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>0334IS01EN-01I2019</t>
+  </si>
+  <si>
+    <t>011MK05PS-33I2019</t>
+  </si>
+  <si>
+    <t>006MK05PS-37I2019</t>
+  </si>
+  <si>
+    <t>OMS 010MK05PS-37I2019</t>
+  </si>
+  <si>
+    <t>018MK05PS-37II2019</t>
+  </si>
+  <si>
+    <t>UMB 0113MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>023MK05PS-33II2019</t>
+  </si>
+  <si>
+    <t>021MK05PS-33II2019</t>
+  </si>
+  <si>
+    <t>025MK05PS-33II2019</t>
+  </si>
+  <si>
+    <t>0132MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>021MK05PS-37II2019</t>
+  </si>
+  <si>
+    <t>0136MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>0137MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>0102MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>019MK05PS-33II2019</t>
+  </si>
+  <si>
+    <t>014MK05PS-37II2019</t>
+  </si>
+  <si>
+    <t>013MK05PS-37II2019</t>
+  </si>
+  <si>
+    <t>016MK05PS-37II2019</t>
+  </si>
+  <si>
+    <t>015MK05PS-37II2019</t>
+  </si>
+  <si>
+    <t>0110MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>017MK05PS-37II2019</t>
+  </si>
+  <si>
+    <t>019MK05PS-37II2019</t>
+  </si>
+  <si>
+    <t>0118MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>023MK05PS-03II2019</t>
+  </si>
+  <si>
+    <t>024MK05PS-03II2019</t>
+  </si>
+  <si>
+    <t>020MK05PS-37II2019</t>
+  </si>
+  <si>
+    <t>093MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>090MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>088MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>089MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>017MK05PS-03I2019</t>
+  </si>
+  <si>
+    <t>015MK05PS-33I2019</t>
+  </si>
+  <si>
+    <t>077MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>073MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>01438MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>023MK05PS-37II2019</t>
+  </si>
+  <si>
+    <t>030MK05PS-33II2019</t>
+  </si>
+  <si>
+    <t>049MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>0155MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>0158MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>064MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>003MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>065MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>052MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>048MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>047MK05PS-05I2019</t>
+  </si>
+  <si>
+    <t>004SV05CM-61I2019</t>
+  </si>
+  <si>
+    <t>008SV05CM-61I2019</t>
+  </si>
+  <si>
+    <t>005SV05CM-61I2019</t>
+  </si>
+  <si>
+    <t>008MK05PS-03I2019</t>
+  </si>
+  <si>
+    <t>001MK05PS-03I2019</t>
+  </si>
+  <si>
+    <t>009MK05PS-33I2019</t>
+  </si>
+  <si>
+    <t>003MK05PS-37I2019</t>
+  </si>
+  <si>
+    <t>010MK05PS-33I2019</t>
+  </si>
+  <si>
+    <t>012MK05PS-33I2019</t>
+  </si>
+  <si>
+    <t>009MK05PS-37I2019</t>
+  </si>
+  <si>
+    <t>005MK05PS-37I2019</t>
+  </si>
+  <si>
+    <t>007MK05PS-33I2019</t>
+  </si>
+  <si>
+    <t>006MK05PS-33I2019</t>
+  </si>
+  <si>
+    <t>001MK05PS-33I2019</t>
+  </si>
+  <si>
+    <t>014MK05PS-33I2019</t>
+  </si>
+  <si>
+    <t>013MK05PS-33I2019</t>
+  </si>
+  <si>
+    <t>008MK05PS-33I2019</t>
+  </si>
+  <si>
+    <t>007MK05PS-37I2019</t>
+  </si>
+  <si>
+    <t>008MK05PS-37I2019</t>
+  </si>
+  <si>
+    <t>031MK05PS-33II2019</t>
+  </si>
+  <si>
+    <t>0169MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>0170MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>0171MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>028MK05PS-03II2019</t>
+  </si>
+  <si>
+    <t>033MK05PS-33II2019</t>
+  </si>
+  <si>
+    <t>029MK05PS-03II2019</t>
+  </si>
+  <si>
+    <t>037MK05PS-33II2019</t>
+  </si>
+  <si>
+    <t>0192MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>032MK05PS-03II2019</t>
+  </si>
+  <si>
+    <t>031MK05PS-03II2019</t>
+  </si>
+  <si>
+    <t>0197MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>042MK05PS-33II2019</t>
+  </si>
+  <si>
+    <t>034MK05PS-03II2019</t>
+  </si>
+  <si>
+    <t>0208MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>027MK05PS-37II2019</t>
+  </si>
+  <si>
+    <t>016SV05CM-61II2019</t>
+  </si>
+  <si>
+    <t>017SV05CM-61II2019</t>
+  </si>
+  <si>
+    <t>0214MK05PS-05II2019</t>
+  </si>
+  <si>
+    <t>048MK05MK-01II2019</t>
+  </si>
+  <si>
+    <t>045MK05PS-33III2019</t>
+  </si>
+  <si>
+    <t>0225MK05PS-05III2019</t>
+  </si>
+  <si>
+    <t>028MK05PS-37III2019</t>
+  </si>
+  <si>
+    <t>0224MK05PS-05III2019</t>
+  </si>
+  <si>
+    <t>046MK05PS-33III2019</t>
+  </si>
+  <si>
+    <t>050MK05PS-33III2019</t>
+  </si>
+  <si>
+    <t>024IS01IY-04III2019</t>
+  </si>
+  <si>
+    <t>052MK05PS-33III2019</t>
+  </si>
+  <si>
+    <t>049MK05PS-33III2019</t>
+  </si>
+  <si>
+    <t>0234MK05PS-05III2019</t>
+  </si>
+  <si>
+    <t>053MK05PS-33III2019</t>
+  </si>
+  <si>
+    <t>0236MK05PS-05III2019</t>
+  </si>
+  <si>
+    <t>038MK05PS-03III2019</t>
+  </si>
+  <si>
+    <t>054MK05PS-33III2019</t>
+  </si>
+  <si>
+    <t>031MK05PS-37III2019</t>
+  </si>
+  <si>
+    <t>057MK05PS-33III2019</t>
+  </si>
+  <si>
+    <t>056MK05PS-33III2019</t>
+  </si>
+  <si>
+    <t>055MK05PS-33III2019</t>
+  </si>
+  <si>
+    <t>032MK05PS-37III2019</t>
+  </si>
+  <si>
+    <t>0243MK05PS-05III2019</t>
+  </si>
+  <si>
+    <t>0246MK05PS-05III2019</t>
+  </si>
+  <si>
+    <t>034MK05PS-37III2019</t>
+  </si>
+  <si>
+    <t>033MK05PS-37III2019</t>
+  </si>
+  <si>
+    <t>0251MK05PS-05III2019</t>
+  </si>
+  <si>
+    <t>059MK05PS-33III2019</t>
+  </si>
+  <si>
+    <t>060MK05PS-33III2019</t>
+  </si>
+  <si>
+    <t>035MK05PS-37III2019</t>
+  </si>
+  <si>
+    <t>041MK05PS-03III2019</t>
+  </si>
+  <si>
+    <t>0270MK05PS-05III2019</t>
+  </si>
+  <si>
+    <t>0269MK05PS-05III2019</t>
+  </si>
+  <si>
+    <t>020SV05CM-61III2019</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J99"/>
+  <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1348,22 +1567,22 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="D2" s="2">
         <v>43480</v>
       </c>
       <c r="F2" t="s">
-        <v>206</v>
+        <v>254</v>
       </c>
       <c r="G2" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
       <c r="I2" t="s">
-        <v>211</v>
+        <v>259</v>
       </c>
       <c r="J2" t="s">
-        <v>215</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1374,22 +1593,22 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="D3" s="2">
         <v>43480</v>
       </c>
       <c r="F3" t="s">
-        <v>206</v>
+        <v>254</v>
       </c>
       <c r="G3" t="s">
-        <v>209</v>
+        <v>257</v>
       </c>
       <c r="I3" t="s">
-        <v>212</v>
+        <v>260</v>
       </c>
       <c r="J3" t="s">
-        <v>216</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1400,16 +1619,16 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="D4" s="2">
         <v>43481</v>
       </c>
       <c r="F4" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J4" t="s">
-        <v>217</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1420,16 +1639,16 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="D5" s="2">
         <v>43481</v>
       </c>
       <c r="F5" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J5" t="s">
-        <v>218</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1440,19 +1659,19 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="D6" s="2">
         <v>43483</v>
       </c>
       <c r="F6" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="I6" t="s">
-        <v>213</v>
+        <v>261</v>
       </c>
       <c r="J6" t="s">
-        <v>219</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1463,19 +1682,19 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="D7" s="2">
         <v>43487</v>
       </c>
       <c r="F7" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="G7" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="J7" t="s">
-        <v>220</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1486,16 +1705,16 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="D8" s="2">
         <v>43493</v>
       </c>
       <c r="F8" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J8" t="s">
-        <v>221</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1506,16 +1725,16 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="D9" s="2">
         <v>43510</v>
       </c>
       <c r="F9" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J9" t="s">
-        <v>222</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1526,16 +1745,16 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="D10" s="2">
         <v>43510</v>
       </c>
       <c r="F10" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J10" t="s">
-        <v>223</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1546,16 +1765,16 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="D11" s="2">
         <v>43510</v>
       </c>
       <c r="F11" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J11" t="s">
-        <v>224</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1566,16 +1785,16 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="D12" s="2">
         <v>43510</v>
       </c>
       <c r="F12" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J12" t="s">
-        <v>225</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1586,16 +1805,16 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="D13" s="2">
         <v>43510</v>
       </c>
       <c r="F13" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J13" t="s">
-        <v>226</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1606,16 +1825,16 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="D14" s="2">
         <v>43510</v>
       </c>
       <c r="F14" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J14" t="s">
-        <v>227</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1626,16 +1845,16 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="D15" s="2">
         <v>43510</v>
       </c>
       <c r="F15" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J15" t="s">
-        <v>228</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1646,16 +1865,16 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="D16" s="2">
         <v>43510</v>
       </c>
       <c r="F16" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J16" t="s">
-        <v>229</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1666,16 +1885,16 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="D17" s="2">
         <v>43510</v>
       </c>
       <c r="F17" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J17" t="s">
-        <v>230</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1686,16 +1905,16 @@
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="D18" s="2">
         <v>43510</v>
       </c>
       <c r="F18" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J18" t="s">
-        <v>231</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1706,16 +1925,16 @@
         <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="D19" s="2">
         <v>43510</v>
       </c>
       <c r="F19" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J19" t="s">
-        <v>232</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1726,16 +1945,16 @@
         <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="D20" s="2">
         <v>43510</v>
       </c>
       <c r="F20" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J20" t="s">
-        <v>233</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1746,16 +1965,16 @@
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="D21" s="2">
         <v>43510</v>
       </c>
       <c r="F21" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J21" t="s">
-        <v>234</v>
+        <v>282</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1766,16 +1985,16 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="D22" s="2">
         <v>43510</v>
       </c>
       <c r="F22" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J22" t="s">
-        <v>235</v>
+        <v>283</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1786,16 +2005,16 @@
         <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="D23" s="2">
         <v>43510</v>
       </c>
       <c r="F23" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J23" t="s">
-        <v>236</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1806,16 +2025,16 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="D24" s="2">
         <v>43510</v>
       </c>
       <c r="F24" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J24" t="s">
-        <v>237</v>
+        <v>285</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1826,16 +2045,16 @@
         <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="D25" s="2">
         <v>43510</v>
       </c>
       <c r="F25" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J25" t="s">
-        <v>238</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1846,16 +2065,16 @@
         <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="D26" s="2">
         <v>43510</v>
       </c>
       <c r="F26" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J26" t="s">
-        <v>239</v>
+        <v>287</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1866,16 +2085,16 @@
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="D27" s="2">
         <v>43510</v>
       </c>
       <c r="F27" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J27" t="s">
-        <v>240</v>
+        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1886,16 +2105,16 @@
         <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="D28" s="2">
         <v>43510</v>
       </c>
       <c r="F28" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J28" t="s">
-        <v>241</v>
+        <v>289</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1906,16 +2125,16 @@
         <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="D29" s="2">
         <v>43510</v>
       </c>
       <c r="F29" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J29" t="s">
-        <v>242</v>
+        <v>290</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1926,16 +2145,16 @@
         <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="D30" s="2">
         <v>43510</v>
       </c>
       <c r="F30" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J30" t="s">
-        <v>243</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1946,16 +2165,16 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="D31" s="2">
         <v>43510</v>
       </c>
       <c r="F31" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J31" t="s">
-        <v>244</v>
+        <v>292</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1966,16 +2185,16 @@
         <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="D32" s="2">
         <v>43510</v>
       </c>
       <c r="F32" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J32" t="s">
-        <v>245</v>
+        <v>293</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1986,16 +2205,16 @@
         <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="D33" s="2">
         <v>43510</v>
       </c>
       <c r="F33" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J33" t="s">
-        <v>246</v>
+        <v>294</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2006,16 +2225,16 @@
         <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="D34" s="2">
         <v>43510</v>
       </c>
       <c r="F34" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J34" t="s">
-        <v>247</v>
+        <v>295</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2026,16 +2245,16 @@
         <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="D35" s="2">
         <v>43510</v>
       </c>
       <c r="F35" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J35" t="s">
-        <v>248</v>
+        <v>296</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2046,16 +2265,16 @@
         <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
       <c r="D36" s="2">
         <v>43510</v>
       </c>
       <c r="F36" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J36" t="s">
-        <v>249</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2066,16 +2285,16 @@
         <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="D37" s="2">
         <v>43510</v>
       </c>
       <c r="F37" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J37" t="s">
-        <v>250</v>
+        <v>298</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2086,16 +2305,16 @@
         <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="D38" s="2">
         <v>43511</v>
       </c>
       <c r="F38" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J38" t="s">
-        <v>251</v>
+        <v>299</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2106,16 +2325,16 @@
         <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="D39" s="2">
         <v>43511</v>
       </c>
       <c r="F39" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J39" t="s">
-        <v>252</v>
+        <v>300</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2126,16 +2345,16 @@
         <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="D40" s="2">
         <v>43511</v>
       </c>
       <c r="F40" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J40" t="s">
-        <v>253</v>
+        <v>301</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2146,22 +2365,22 @@
         <v>49</v>
       </c>
       <c r="C41" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="D41" s="2">
         <v>43511</v>
       </c>
       <c r="F41" t="s">
-        <v>206</v>
+        <v>254</v>
       </c>
       <c r="G41" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="I41" t="s">
-        <v>214</v>
+        <v>262</v>
       </c>
       <c r="J41" t="s">
-        <v>254</v>
+        <v>302</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2172,16 +2391,16 @@
         <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="D42" s="2">
         <v>43511</v>
       </c>
       <c r="F42" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J42" t="s">
-        <v>50</v>
+        <v>303</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2192,16 +2411,16 @@
         <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="D43" s="2">
         <v>43511</v>
       </c>
       <c r="F43" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J43" t="s">
-        <v>255</v>
+        <v>304</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2212,16 +2431,16 @@
         <v>52</v>
       </c>
       <c r="C44" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="D44" s="2">
         <v>43511</v>
       </c>
       <c r="F44" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J44" t="s">
-        <v>256</v>
+        <v>305</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2232,16 +2451,16 @@
         <v>53</v>
       </c>
       <c r="C45" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="D45" s="2">
         <v>43511</v>
       </c>
       <c r="F45" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J45" t="s">
-        <v>257</v>
+        <v>306</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2252,16 +2471,16 @@
         <v>54</v>
       </c>
       <c r="C46" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="D46" s="2">
         <v>43511</v>
       </c>
       <c r="F46" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J46" t="s">
-        <v>258</v>
+        <v>307</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2272,16 +2491,16 @@
         <v>55</v>
       </c>
       <c r="C47" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="D47" s="2">
         <v>43511</v>
       </c>
       <c r="F47" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J47" t="s">
-        <v>259</v>
+        <v>308</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2292,16 +2511,16 @@
         <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="D48" s="2">
         <v>43511</v>
       </c>
       <c r="F48" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J48" t="s">
-        <v>260</v>
+        <v>309</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2312,16 +2531,16 @@
         <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="D49" s="2">
         <v>43511</v>
       </c>
       <c r="F49" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J49" t="s">
-        <v>261</v>
+        <v>310</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2332,16 +2551,16 @@
         <v>58</v>
       </c>
       <c r="C50" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="D50" s="2">
         <v>43511</v>
       </c>
       <c r="F50" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J50" t="s">
-        <v>262</v>
+        <v>311</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2352,16 +2571,16 @@
         <v>59</v>
       </c>
       <c r="C51" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="D51" s="2">
         <v>43511</v>
       </c>
       <c r="F51" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J51" t="s">
-        <v>263</v>
+        <v>312</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2372,16 +2591,16 @@
         <v>60</v>
       </c>
       <c r="C52" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="D52" s="2">
         <v>43511</v>
       </c>
       <c r="F52" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J52" t="s">
-        <v>264</v>
+        <v>313</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2392,16 +2611,16 @@
         <v>61</v>
       </c>
       <c r="C53" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="D53" s="2">
         <v>43511</v>
       </c>
       <c r="F53" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J53" t="s">
-        <v>265</v>
+        <v>314</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2412,16 +2631,16 @@
         <v>62</v>
       </c>
       <c r="C54" t="s">
-        <v>160</v>
+        <v>184</v>
       </c>
       <c r="D54" s="2">
         <v>43511</v>
       </c>
       <c r="F54" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J54" t="s">
-        <v>266</v>
+        <v>315</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2432,16 +2651,16 @@
         <v>63</v>
       </c>
       <c r="C55" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="D55" s="2">
         <v>43511</v>
       </c>
       <c r="F55" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J55" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2452,16 +2671,16 @@
         <v>64</v>
       </c>
       <c r="C56" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="D56" s="2">
         <v>43511</v>
       </c>
       <c r="F56" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J56" t="s">
-        <v>268</v>
+        <v>317</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2472,16 +2691,16 @@
         <v>65</v>
       </c>
       <c r="C57" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="D57" s="2">
         <v>43511</v>
       </c>
       <c r="F57" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J57" t="s">
-        <v>269</v>
+        <v>318</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2492,16 +2711,16 @@
         <v>66</v>
       </c>
       <c r="C58" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="D58" s="2">
         <v>43511</v>
       </c>
       <c r="F58" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J58" t="s">
-        <v>270</v>
+        <v>319</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2512,16 +2731,16 @@
         <v>67</v>
       </c>
       <c r="C59" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="D59" s="2">
         <v>43511</v>
       </c>
       <c r="F59" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J59" t="s">
-        <v>271</v>
+        <v>320</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2532,16 +2751,16 @@
         <v>68</v>
       </c>
       <c r="C60" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="D60" s="2">
         <v>43511</v>
       </c>
       <c r="F60" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J60" t="s">
-        <v>272</v>
+        <v>321</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -2552,16 +2771,16 @@
         <v>69</v>
       </c>
       <c r="C61" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="D61" s="2">
         <v>43511</v>
       </c>
       <c r="F61" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J61" t="s">
-        <v>273</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2572,16 +2791,16 @@
         <v>70</v>
       </c>
       <c r="C62" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="D62" s="2">
         <v>43511</v>
       </c>
       <c r="F62" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J62" t="s">
-        <v>274</v>
+        <v>323</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2592,16 +2811,16 @@
         <v>71</v>
       </c>
       <c r="C63" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
       <c r="D63" s="2">
         <v>43511</v>
       </c>
       <c r="F63" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J63" t="s">
-        <v>275</v>
+        <v>324</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2612,16 +2831,16 @@
         <v>72</v>
       </c>
       <c r="C64" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="D64" s="2">
         <v>43511</v>
       </c>
       <c r="F64" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J64" t="s">
-        <v>276</v>
+        <v>325</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -2632,16 +2851,16 @@
         <v>73</v>
       </c>
       <c r="C65" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="D65" s="2">
         <v>43511</v>
       </c>
       <c r="F65" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J65" t="s">
-        <v>277</v>
+        <v>326</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -2652,16 +2871,16 @@
         <v>74</v>
       </c>
       <c r="C66" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="D66" s="2">
         <v>43511</v>
       </c>
       <c r="F66" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J66" t="s">
-        <v>278</v>
+        <v>327</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2672,16 +2891,16 @@
         <v>75</v>
       </c>
       <c r="C67" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="D67" s="2">
         <v>43511</v>
       </c>
       <c r="F67" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J67" t="s">
-        <v>279</v>
+        <v>328</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -2692,16 +2911,16 @@
         <v>76</v>
       </c>
       <c r="C68" t="s">
-        <v>174</v>
+        <v>198</v>
       </c>
       <c r="D68" s="2">
         <v>43511</v>
       </c>
       <c r="F68" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J68" t="s">
-        <v>280</v>
+        <v>329</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -2712,16 +2931,16 @@
         <v>77</v>
       </c>
       <c r="C69" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="D69" s="2">
         <v>43512.02811368056</v>
       </c>
       <c r="F69" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J69" t="s">
-        <v>281</v>
+        <v>330</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -2732,16 +2951,16 @@
         <v>78</v>
       </c>
       <c r="C70" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="D70" s="2">
         <v>43514.58475023148</v>
       </c>
       <c r="F70" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J70" t="s">
-        <v>282</v>
+        <v>331</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -2752,16 +2971,16 @@
         <v>79</v>
       </c>
       <c r="C71" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="D71" s="2">
         <v>43514.58475289352</v>
       </c>
       <c r="F71" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J71" t="s">
-        <v>283</v>
+        <v>332</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -2772,16 +2991,16 @@
         <v>80</v>
       </c>
       <c r="C72" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="D72" s="2">
         <v>43514.58475601852</v>
       </c>
       <c r="F72" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J72" t="s">
-        <v>284</v>
+        <v>333</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -2792,16 +3011,16 @@
         <v>81</v>
       </c>
       <c r="C73" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="D73" s="2">
         <v>43514.58475809028</v>
       </c>
       <c r="F73" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J73" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -2812,16 +3031,16 @@
         <v>82</v>
       </c>
       <c r="C74" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="D74" s="2">
         <v>43515.48238950231</v>
       </c>
       <c r="F74" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J74" t="s">
-        <v>286</v>
+        <v>335</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -2832,16 +3051,16 @@
         <v>83</v>
       </c>
       <c r="C75" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="D75" s="2">
         <v>43515.73058116898</v>
       </c>
       <c r="F75" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J75" t="s">
-        <v>287</v>
+        <v>336</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -2852,16 +3071,16 @@
         <v>84</v>
       </c>
       <c r="C76" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="D76" s="2">
         <v>43515.73058324074</v>
       </c>
       <c r="F76" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J76" t="s">
-        <v>288</v>
+        <v>337</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -2872,16 +3091,16 @@
         <v>85</v>
       </c>
       <c r="C77" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="D77" s="2">
         <v>43516.4953059375</v>
       </c>
       <c r="F77" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J77" t="s">
-        <v>289</v>
+        <v>338</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -2892,16 +3111,16 @@
         <v>86</v>
       </c>
       <c r="C78" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="D78" s="2">
         <v>43518.61259846065</v>
       </c>
       <c r="F78" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J78" t="s">
-        <v>290</v>
+        <v>339</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -2912,16 +3131,16 @@
         <v>87</v>
       </c>
       <c r="C79" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="D79" s="2">
         <v>43521.6215687037</v>
       </c>
       <c r="F79" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J79" t="s">
-        <v>291</v>
+        <v>340</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -2932,16 +3151,16 @@
         <v>88</v>
       </c>
       <c r="C80" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="D80" s="2">
         <v>43521.6215702662</v>
       </c>
       <c r="F80" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J80" t="s">
-        <v>292</v>
+        <v>341</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -2952,16 +3171,16 @@
         <v>89</v>
       </c>
       <c r="C81" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="D81" s="2">
         <v>43521.6215747338</v>
       </c>
       <c r="F81" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J81" t="s">
-        <v>293</v>
+        <v>342</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -2972,16 +3191,16 @@
         <v>90</v>
       </c>
       <c r="C82" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="D82" s="2">
         <v>43521.6215747338</v>
       </c>
       <c r="F82" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J82" t="s">
-        <v>294</v>
+        <v>343</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -2992,16 +3211,16 @@
         <v>91</v>
       </c>
       <c r="C83" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="D83" s="2">
         <v>43522.71610519676</v>
       </c>
       <c r="F83" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J83" t="s">
-        <v>295</v>
+        <v>344</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -3012,16 +3231,16 @@
         <v>92</v>
       </c>
       <c r="C84" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D84" s="2">
         <v>43522.71610894676</v>
       </c>
       <c r="F84" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J84" t="s">
-        <v>296</v>
+        <v>345</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -3032,16 +3251,16 @@
         <v>93</v>
       </c>
       <c r="C85" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="D85" s="2">
         <v>43523.38975456019</v>
       </c>
       <c r="F85" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J85" t="s">
-        <v>297</v>
+        <v>346</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -3052,16 +3271,16 @@
         <v>94</v>
       </c>
       <c r="C86" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="D86" s="2">
         <v>43524.45939690972</v>
       </c>
       <c r="F86" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J86" t="s">
-        <v>298</v>
+        <v>347</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -3072,16 +3291,16 @@
         <v>95</v>
       </c>
       <c r="C87" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="D87" s="2">
         <v>43524.45991893519</v>
       </c>
       <c r="F87" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J87" t="s">
-        <v>299</v>
+        <v>348</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -3092,16 +3311,16 @@
         <v>96</v>
       </c>
       <c r="C88" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="D88" s="2">
         <v>43524.45991893519</v>
       </c>
       <c r="F88" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J88" t="s">
-        <v>300</v>
+        <v>349</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -3112,16 +3331,16 @@
         <v>97</v>
       </c>
       <c r="C89" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="D89" s="2">
         <v>43524.45991893519</v>
       </c>
       <c r="F89" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J89" t="s">
-        <v>301</v>
+        <v>350</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -3132,16 +3351,16 @@
         <v>98</v>
       </c>
       <c r="C90" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="D90" s="2">
         <v>43529.37632800926</v>
       </c>
       <c r="F90" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J90" t="s">
-        <v>302</v>
+        <v>351</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -3152,16 +3371,16 @@
         <v>99</v>
       </c>
       <c r="C91" t="s">
-        <v>197</v>
+        <v>221</v>
       </c>
       <c r="D91" s="2">
         <v>43529.37633297453</v>
       </c>
       <c r="F91" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J91" t="s">
-        <v>303</v>
+        <v>352</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -3172,16 +3391,16 @@
         <v>100</v>
       </c>
       <c r="C92" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="D92" s="2">
         <v>43529.42497050926</v>
       </c>
       <c r="F92" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J92" t="s">
-        <v>304</v>
+        <v>353</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -3192,16 +3411,16 @@
         <v>101</v>
       </c>
       <c r="C93" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
       <c r="D93" s="2">
         <v>43529.42497885416</v>
       </c>
       <c r="F93" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J93" t="s">
-        <v>305</v>
+        <v>354</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -3212,16 +3431,16 @@
         <v>102</v>
       </c>
       <c r="C94" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="D94" s="2">
         <v>43529.48534415509</v>
       </c>
       <c r="F94" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J94" t="s">
-        <v>306</v>
+        <v>355</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -3232,16 +3451,16 @@
         <v>103</v>
       </c>
       <c r="C95" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="D95" s="2">
         <v>43529.74539105324</v>
       </c>
       <c r="F95" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J95" t="s">
-        <v>307</v>
+        <v>356</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -3252,19 +3471,19 @@
         <v>104</v>
       </c>
       <c r="C96" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="D96" s="2">
         <v>43529.75238363426</v>
       </c>
       <c r="F96" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="J96" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
       <c r="A97">
         <v>8</v>
       </c>
@@ -3272,16 +3491,19 @@
         <v>105</v>
       </c>
       <c r="C97" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="D97" s="2">
         <v>43529.7523853125</v>
       </c>
       <c r="F97" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
+        <v>255</v>
+      </c>
+      <c r="J97" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
       <c r="A98">
         <v>9</v>
       </c>
@@ -3289,16 +3511,19 @@
         <v>106</v>
       </c>
       <c r="C98" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="D98" s="2">
         <v>43529.79556278935</v>
       </c>
       <c r="F98" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
+        <v>255</v>
+      </c>
+      <c r="J98" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
       <c r="A99">
         <v>10</v>
       </c>
@@ -3306,13 +3531,487 @@
         <v>107</v>
       </c>
       <c r="C99" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="D99" s="2">
-        <v>43530.39331518118</v>
+        <v>43530.39331518518</v>
       </c>
       <c r="F99" t="s">
-        <v>207</v>
+        <v>255</v>
+      </c>
+      <c r="J99" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100">
+        <v>11</v>
+      </c>
+      <c r="B100" t="s">
+        <v>108</v>
+      </c>
+      <c r="C100" t="s">
+        <v>230</v>
+      </c>
+      <c r="D100" s="2">
+        <v>43530.81668289352</v>
+      </c>
+      <c r="F100" t="s">
+        <v>255</v>
+      </c>
+      <c r="J100" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101">
+        <v>12</v>
+      </c>
+      <c r="B101" t="s">
+        <v>109</v>
+      </c>
+      <c r="C101" t="s">
+        <v>231</v>
+      </c>
+      <c r="D101" s="2">
+        <v>43530.81669511574</v>
+      </c>
+      <c r="F101" t="s">
+        <v>255</v>
+      </c>
+      <c r="J101" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102">
+        <v>13</v>
+      </c>
+      <c r="B102" t="s">
+        <v>110</v>
+      </c>
+      <c r="C102" t="s">
+        <v>232</v>
+      </c>
+      <c r="D102" s="2">
+        <v>43532.40770633102</v>
+      </c>
+      <c r="F102" t="s">
+        <v>255</v>
+      </c>
+      <c r="J102" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103">
+        <v>14</v>
+      </c>
+      <c r="B103" t="s">
+        <v>111</v>
+      </c>
+      <c r="C103" t="s">
+        <v>233</v>
+      </c>
+      <c r="D103" s="2">
+        <v>43532.40898523148</v>
+      </c>
+      <c r="F103" t="s">
+        <v>255</v>
+      </c>
+      <c r="J103" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104">
+        <v>15</v>
+      </c>
+      <c r="B104" t="s">
+        <v>112</v>
+      </c>
+      <c r="C104" t="s">
+        <v>234</v>
+      </c>
+      <c r="D104" s="2">
+        <v>43532.59223354167</v>
+      </c>
+      <c r="F104" t="s">
+        <v>255</v>
+      </c>
+      <c r="J104" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105">
+        <v>16</v>
+      </c>
+      <c r="B105" t="s">
+        <v>113</v>
+      </c>
+      <c r="C105" t="s">
+        <v>235</v>
+      </c>
+      <c r="D105" s="2">
+        <v>43535.35740248843</v>
+      </c>
+      <c r="F105" t="s">
+        <v>255</v>
+      </c>
+      <c r="J105" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106">
+        <v>17</v>
+      </c>
+      <c r="B106" t="s">
+        <v>114</v>
+      </c>
+      <c r="C106" t="s">
+        <v>236</v>
+      </c>
+      <c r="D106" s="2">
+        <v>43535.35740469908</v>
+      </c>
+      <c r="F106" t="s">
+        <v>255</v>
+      </c>
+      <c r="J106" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107">
+        <v>18</v>
+      </c>
+      <c r="B107" t="s">
+        <v>115</v>
+      </c>
+      <c r="C107" t="s">
+        <v>237</v>
+      </c>
+      <c r="D107" s="2">
+        <v>43535.35740587963</v>
+      </c>
+      <c r="F107" t="s">
+        <v>255</v>
+      </c>
+      <c r="J107" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="A108">
+        <v>19</v>
+      </c>
+      <c r="B108" t="s">
+        <v>116</v>
+      </c>
+      <c r="C108" t="s">
+        <v>238</v>
+      </c>
+      <c r="D108" s="2">
+        <v>43535.35740699074</v>
+      </c>
+      <c r="F108" t="s">
+        <v>255</v>
+      </c>
+      <c r="J108" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109">
+        <v>20</v>
+      </c>
+      <c r="B109" t="s">
+        <v>117</v>
+      </c>
+      <c r="C109" t="s">
+        <v>239</v>
+      </c>
+      <c r="D109" s="2">
+        <v>43535.35741133102</v>
+      </c>
+      <c r="F109" t="s">
+        <v>255</v>
+      </c>
+      <c r="J109" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
+      <c r="A110">
+        <v>21</v>
+      </c>
+      <c r="B110" t="s">
+        <v>118</v>
+      </c>
+      <c r="C110" t="s">
+        <v>240</v>
+      </c>
+      <c r="D110" s="2">
+        <v>43535.35741549769</v>
+      </c>
+      <c r="F110" t="s">
+        <v>255</v>
+      </c>
+      <c r="J110" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111">
+        <v>22</v>
+      </c>
+      <c r="B111" t="s">
+        <v>119</v>
+      </c>
+      <c r="C111" t="s">
+        <v>241</v>
+      </c>
+      <c r="D111" s="2">
+        <v>43535.69687207176</v>
+      </c>
+      <c r="F111" t="s">
+        <v>255</v>
+      </c>
+      <c r="J111" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
+      <c r="A112">
+        <v>23</v>
+      </c>
+      <c r="B112" t="s">
+        <v>120</v>
+      </c>
+      <c r="C112" t="s">
+        <v>242</v>
+      </c>
+      <c r="D112" s="2">
+        <v>43535.69687763889</v>
+      </c>
+      <c r="F112" t="s">
+        <v>255</v>
+      </c>
+      <c r="J112" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="A113">
+        <v>24</v>
+      </c>
+      <c r="B113" t="s">
+        <v>121</v>
+      </c>
+      <c r="C113" t="s">
+        <v>243</v>
+      </c>
+      <c r="D113" s="2">
+        <v>43535.72659671296</v>
+      </c>
+      <c r="F113" t="s">
+        <v>255</v>
+      </c>
+      <c r="J113" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
+      <c r="A114">
+        <v>25</v>
+      </c>
+      <c r="B114" t="s">
+        <v>122</v>
+      </c>
+      <c r="C114" t="s">
+        <v>244</v>
+      </c>
+      <c r="D114" s="2">
+        <v>43537.40848363426</v>
+      </c>
+      <c r="F114" t="s">
+        <v>255</v>
+      </c>
+      <c r="J114" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="A115">
+        <v>26</v>
+      </c>
+      <c r="B115" t="s">
+        <v>123</v>
+      </c>
+      <c r="C115" t="s">
+        <v>245</v>
+      </c>
+      <c r="D115" s="2">
+        <v>43538.43785037037</v>
+      </c>
+      <c r="F115" t="s">
+        <v>255</v>
+      </c>
+      <c r="J115" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116">
+        <v>27</v>
+      </c>
+      <c r="B116" t="s">
+        <v>124</v>
+      </c>
+      <c r="C116" t="s">
+        <v>246</v>
+      </c>
+      <c r="D116" s="2">
+        <v>43538.45286440972</v>
+      </c>
+      <c r="F116" t="s">
+        <v>255</v>
+      </c>
+      <c r="J116" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117">
+        <v>28</v>
+      </c>
+      <c r="B117" t="s">
+        <v>125</v>
+      </c>
+      <c r="C117" t="s">
+        <v>247</v>
+      </c>
+      <c r="D117" s="2">
+        <v>43539.3654228588</v>
+      </c>
+      <c r="F117" t="s">
+        <v>255</v>
+      </c>
+      <c r="J117" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118">
+        <v>29</v>
+      </c>
+      <c r="B118" t="s">
+        <v>126</v>
+      </c>
+      <c r="C118" t="s">
+        <v>248</v>
+      </c>
+      <c r="D118" s="2">
+        <v>43542.56313657408</v>
+      </c>
+      <c r="F118" t="s">
+        <v>255</v>
+      </c>
+      <c r="J118" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119">
+        <v>30</v>
+      </c>
+      <c r="B119" t="s">
+        <v>127</v>
+      </c>
+      <c r="C119" t="s">
+        <v>249</v>
+      </c>
+      <c r="D119" s="2">
+        <v>43542.56314506944</v>
+      </c>
+      <c r="F119" t="s">
+        <v>255</v>
+      </c>
+      <c r="J119" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10">
+      <c r="A120">
+        <v>31</v>
+      </c>
+      <c r="B120" t="s">
+        <v>128</v>
+      </c>
+      <c r="C120" t="s">
+        <v>250</v>
+      </c>
+      <c r="D120" s="2">
+        <v>43542.56314643518</v>
+      </c>
+      <c r="F120" t="s">
+        <v>255</v>
+      </c>
+      <c r="J120" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
+      <c r="A121">
+        <v>32</v>
+      </c>
+      <c r="B121" t="s">
+        <v>129</v>
+      </c>
+      <c r="C121" t="s">
+        <v>251</v>
+      </c>
+      <c r="D121" s="2">
+        <v>43543.55330482867</v>
+      </c>
+      <c r="F121" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
+      <c r="A122">
+        <v>33</v>
+      </c>
+      <c r="B122" t="s">
+        <v>130</v>
+      </c>
+      <c r="C122" t="s">
+        <v>252</v>
+      </c>
+      <c r="D122" s="2">
+        <v>43543.55330563703</v>
+      </c>
+      <c r="F122" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
+      <c r="A123">
+        <v>34</v>
+      </c>
+      <c r="B123" t="s">
+        <v>131</v>
+      </c>
+      <c r="C123" t="s">
+        <v>253</v>
+      </c>
+      <c r="D123" s="2">
+        <v>43543.55330700071</v>
+      </c>
+      <c r="F123" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change write to excel functionality inside while loop, so if any error happen it will still save the excel data
</commit_message>
<xml_diff>
--- a/New Products Assmt.xlsx
+++ b/New Products Assmt.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="427">
   <si>
     <t>No</t>
   </si>
@@ -403,6 +403,9 @@
     <t>020/SV.05/CM-61/III/2019</t>
   </si>
   <si>
+    <t>0287/MK.05/PS-05/III/2019</t>
+  </si>
+  <si>
     <t>066/MK.05/PS-33/III/2019</t>
   </si>
   <si>
@@ -412,6 +415,69 @@
     <t>065/MK.05/PS-33/III/2019</t>
   </si>
   <si>
+    <t>037/MK.05/PS-37/III/2019</t>
+  </si>
+  <si>
+    <t>036/MK.05/PS-37/III/2019</t>
+  </si>
+  <si>
+    <t>068/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>067/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>044/MK.05/PS-03/III/2019</t>
+  </si>
+  <si>
+    <t>045/MK.05/PS-03/III/2019</t>
+  </si>
+  <si>
+    <t>045/MK.05/MK-01/II/2019</t>
+  </si>
+  <si>
+    <t>070/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>072/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>071/MK.05/PS-33/III/2019</t>
+  </si>
+  <si>
+    <t>074/MK.05/PS-33/IV/2019</t>
+  </si>
+  <si>
+    <t>073/MK.05/PS-33/IV/2019</t>
+  </si>
+  <si>
+    <t>075/MK.05/PS-33/IV/2019</t>
+  </si>
+  <si>
+    <t>041/MK.05/PS-37/IV/2019</t>
+  </si>
+  <si>
+    <t>0332/MK.05/PS-05/IV/2019</t>
+  </si>
+  <si>
+    <t>077/MK.05/PS-33/IV/2019</t>
+  </si>
+  <si>
+    <t>040/MK.05/PS-37/IV/2019</t>
+  </si>
+  <si>
+    <t>0345/MK.05/PS-05/IV/2019</t>
+  </si>
+  <si>
+    <t>082/MK.05/PS-33/IV/2019</t>
+  </si>
+  <si>
+    <t>081/MK.05/PS-33/IV/2019</t>
+  </si>
+  <si>
+    <t>0350/MK.05/PS-05/IV/2019</t>
+  </si>
+  <si>
     <t>[Nota Dinas] Permohonan Batch Offer untuk Pelanggan BC 06 per Januari 2019 (005/MK.05/PS-03/I/2019)</t>
   </si>
   <si>
@@ -769,6 +835,9 @@
     <t>[Nota Dinas] Permohonan Pembuatan APN Komersial Corporate PLN  UP2D Jakarta (UP2DTSEL) (020/SV.05/CM-61/III/2019)</t>
   </si>
   <si>
+    <t>[Nota Dinas] Status Kesiapan Komersial (RFC) Paket Surprise Deal MusicMAX (Postpaid) (0287/MK.05/PS-05/III/2019)</t>
+  </si>
+  <si>
     <t>[Nota Dinas] Pemberitahuan RFI Perubahan Notifikasi SMS Roaming di Malaysia (066/MK.05/PS-33/III/2019)</t>
   </si>
   <si>
@@ -776,6 +845,72 @@
   </si>
   <si>
     <t>[Nota Dinas] Pemberitahuan RFI Migration Roaming Prepaid Non-Rollover Ph2 (065/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFS Paket Halo Kick HVC Fast Track (037/MK.05/PS-37/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFI Paket Family Plan Cross Brand – Postpaid Parent (MyTsel) (036/MK.05/PS-37/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RF1 Paket Roaming Prepaid Standalone API Digicore pada UMB (Promo Eropa Amerika, Asia Reguler, Eropa Reguler, Amerika Afrika, dan Haji) (068/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFI Paket Roaming Prepaid Standalone API Digicore pada UMB (Umroh dan Promo Asia Australia) (067/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Permohonan Batch Remove Offer Old CLS kartuHalo B0/Karyawan (044/MK.05/PS-03/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Permohonan Batch Offer Bonus Spesial Migrasi dan Value CLS (045/MK.05/PS-03/III/2019)</t>
+  </si>
+  <si>
+    <t>Sosialisasi Perubahan Basic Tariff Voice Onnet di Madura dan Pantura Stage 1</t>
+  </si>
+  <si>
+    <t>Sosialisasi Program Quick-Win Family Plan</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFI Fixing Postpaid Roaming Standalone Data Consumption Issue (070/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFS Offer Diskon 2000K &amp;amp; 4000K untuk Nomor Test (072/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFS Paket Halo Kick Bank 100K &amp;amp; 150K (071/MK.05/PS-33/III/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFI Fixing Postpaid Capped PAYU Data Roaming Singapore, Malaysia, Oman (074/MK.05/PS-33/IV/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFI Takeout Taiwan, Sri Lanka, Saudi Arabia dari Flat Call 007 (073/MK.05/PS-33/IV/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan Revisi RFS Paket Roamazing (075/MK.05/PS-33/IV/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFS Paket Halo Kick Hybrid Enable (041/MK.05/PS-37/IV/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Status Kesiapan Komersial (RFC) Paket Halo Kick Bank 100K &amp;amp; 150K (0332/MK.05/PS-05/IV/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFS OCS Turbo Charging Site Jakarta (TBS) untuk FUT Postpaid Ph1 PAYU and Basic Service (077/MK.05/PS-33/IV/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan RFI Retail Bundling Samsung S10 (Flexible Offer) (040/MK.05/PS-37/IV/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Status Kesiapan Komersial (RFC) Takeout Taiwan, Sri Lanka, Saudi Arabia dari Flat Call 007 (0345/MK.05/PS-05/IV/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan Revisi RFS OCS Turbo Charging Site Jakarta (TBS) untuk FUT Postpaid Ph1 PAYU and Basic Service (082/MK.05/PS-33/IV/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Pemberitahuan Revisi RFS Paket Halo Kick HVC Bank 550K (OMSKe1Th2019) (081/MK.05/PS-33/IV/2019)</t>
+  </si>
+  <si>
+    <t>[Nota Dinas] Laporan Hasil Inspeksi (ITR)  Takeout Taiwan, Sri Lanka, Saudi Arabia dari Flat Call 007 (0350/MK.05/PS-05/IV/2019)</t>
   </si>
   <si>
     <t>in progress</t>
@@ -1521,7 +1656,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J123"/>
+  <dimension ref="A1:J146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1567,22 +1702,22 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="D2" s="2">
         <v>43480</v>
       </c>
       <c r="F2" t="s">
-        <v>254</v>
+        <v>299</v>
       </c>
       <c r="G2" t="s">
-        <v>256</v>
+        <v>301</v>
       </c>
       <c r="I2" t="s">
-        <v>259</v>
+        <v>304</v>
       </c>
       <c r="J2" t="s">
-        <v>263</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1593,22 +1728,22 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="D3" s="2">
         <v>43480</v>
       </c>
       <c r="F3" t="s">
-        <v>254</v>
+        <v>299</v>
       </c>
       <c r="G3" t="s">
-        <v>257</v>
+        <v>302</v>
       </c>
       <c r="I3" t="s">
-        <v>260</v>
+        <v>305</v>
       </c>
       <c r="J3" t="s">
-        <v>264</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1619,16 +1754,16 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="D4" s="2">
         <v>43481</v>
       </c>
       <c r="F4" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J4" t="s">
-        <v>265</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1639,16 +1774,16 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="D5" s="2">
         <v>43481</v>
       </c>
       <c r="F5" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J5" t="s">
-        <v>266</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1659,19 +1794,19 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="D6" s="2">
         <v>43483</v>
       </c>
       <c r="F6" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="I6" t="s">
-        <v>261</v>
+        <v>306</v>
       </c>
       <c r="J6" t="s">
-        <v>267</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1682,19 +1817,19 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="D7" s="2">
         <v>43487</v>
       </c>
       <c r="F7" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="G7" t="s">
-        <v>258</v>
+        <v>303</v>
       </c>
       <c r="J7" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1705,16 +1840,16 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="D8" s="2">
         <v>43493</v>
       </c>
       <c r="F8" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J8" t="s">
-        <v>269</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1725,16 +1860,16 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="D9" s="2">
         <v>43510</v>
       </c>
       <c r="F9" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J9" t="s">
-        <v>270</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1745,16 +1880,16 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="D10" s="2">
         <v>43510</v>
       </c>
       <c r="F10" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J10" t="s">
-        <v>271</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1765,16 +1900,16 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="D11" s="2">
         <v>43510</v>
       </c>
       <c r="F11" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J11" t="s">
-        <v>272</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1785,16 +1920,16 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="D12" s="2">
         <v>43510</v>
       </c>
       <c r="F12" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J12" t="s">
-        <v>273</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1805,16 +1940,16 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="D13" s="2">
         <v>43510</v>
       </c>
       <c r="F13" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J13" t="s">
-        <v>274</v>
+        <v>319</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1825,16 +1960,16 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="D14" s="2">
         <v>43510</v>
       </c>
       <c r="F14" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J14" t="s">
-        <v>275</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1845,16 +1980,16 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="D15" s="2">
         <v>43510</v>
       </c>
       <c r="F15" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J15" t="s">
-        <v>276</v>
+        <v>321</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1865,16 +2000,16 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="D16" s="2">
         <v>43510</v>
       </c>
       <c r="F16" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J16" t="s">
-        <v>277</v>
+        <v>322</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1885,16 +2020,16 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="D17" s="2">
         <v>43510</v>
       </c>
       <c r="F17" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J17" t="s">
-        <v>278</v>
+        <v>323</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1905,16 +2040,16 @@
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="D18" s="2">
         <v>43510</v>
       </c>
       <c r="F18" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J18" t="s">
-        <v>279</v>
+        <v>324</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1925,16 +2060,16 @@
         <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="D19" s="2">
         <v>43510</v>
       </c>
       <c r="F19" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J19" t="s">
-        <v>280</v>
+        <v>325</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1945,16 +2080,16 @@
         <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="D20" s="2">
         <v>43510</v>
       </c>
       <c r="F20" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J20" t="s">
-        <v>281</v>
+        <v>326</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1965,16 +2100,16 @@
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="D21" s="2">
         <v>43510</v>
       </c>
       <c r="F21" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J21" t="s">
-        <v>282</v>
+        <v>327</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1985,16 +2120,16 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="D22" s="2">
         <v>43510</v>
       </c>
       <c r="F22" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J22" t="s">
-        <v>283</v>
+        <v>328</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2005,16 +2140,16 @@
         <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="D23" s="2">
         <v>43510</v>
       </c>
       <c r="F23" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J23" t="s">
-        <v>284</v>
+        <v>329</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -2025,16 +2160,16 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="D24" s="2">
         <v>43510</v>
       </c>
       <c r="F24" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J24" t="s">
-        <v>285</v>
+        <v>330</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2045,16 +2180,16 @@
         <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>155</v>
+        <v>177</v>
       </c>
       <c r="D25" s="2">
         <v>43510</v>
       </c>
       <c r="F25" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J25" t="s">
-        <v>286</v>
+        <v>331</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -2065,16 +2200,16 @@
         <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="D26" s="2">
         <v>43510</v>
       </c>
       <c r="F26" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J26" t="s">
-        <v>287</v>
+        <v>332</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2085,16 +2220,16 @@
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="D27" s="2">
         <v>43510</v>
       </c>
       <c r="F27" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J27" t="s">
-        <v>288</v>
+        <v>333</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2105,16 +2240,16 @@
         <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="D28" s="2">
         <v>43510</v>
       </c>
       <c r="F28" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J28" t="s">
-        <v>289</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2125,16 +2260,16 @@
         <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="D29" s="2">
         <v>43510</v>
       </c>
       <c r="F29" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J29" t="s">
-        <v>290</v>
+        <v>335</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2145,16 +2280,16 @@
         <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="D30" s="2">
         <v>43510</v>
       </c>
       <c r="F30" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J30" t="s">
-        <v>291</v>
+        <v>336</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2165,16 +2300,16 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="D31" s="2">
         <v>43510</v>
       </c>
       <c r="F31" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J31" t="s">
-        <v>292</v>
+        <v>337</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2185,16 +2320,16 @@
         <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="D32" s="2">
         <v>43510</v>
       </c>
       <c r="F32" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J32" t="s">
-        <v>293</v>
+        <v>338</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2205,16 +2340,16 @@
         <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="D33" s="2">
         <v>43510</v>
       </c>
       <c r="F33" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J33" t="s">
-        <v>294</v>
+        <v>339</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2225,16 +2360,16 @@
         <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="D34" s="2">
         <v>43510</v>
       </c>
       <c r="F34" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J34" t="s">
-        <v>295</v>
+        <v>340</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2245,16 +2380,16 @@
         <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>165</v>
+        <v>187</v>
       </c>
       <c r="D35" s="2">
         <v>43510</v>
       </c>
       <c r="F35" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J35" t="s">
-        <v>296</v>
+        <v>341</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2265,16 +2400,16 @@
         <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>166</v>
+        <v>188</v>
       </c>
       <c r="D36" s="2">
         <v>43510</v>
       </c>
       <c r="F36" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J36" t="s">
-        <v>297</v>
+        <v>342</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2285,16 +2420,16 @@
         <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="D37" s="2">
         <v>43510</v>
       </c>
       <c r="F37" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J37" t="s">
-        <v>298</v>
+        <v>343</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2305,16 +2440,16 @@
         <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
       <c r="D38" s="2">
         <v>43511</v>
       </c>
       <c r="F38" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J38" t="s">
-        <v>299</v>
+        <v>344</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2325,16 +2460,16 @@
         <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>169</v>
+        <v>191</v>
       </c>
       <c r="D39" s="2">
         <v>43511</v>
       </c>
       <c r="F39" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J39" t="s">
-        <v>300</v>
+        <v>345</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2345,16 +2480,16 @@
         <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="D40" s="2">
         <v>43511</v>
       </c>
       <c r="F40" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J40" t="s">
-        <v>301</v>
+        <v>346</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2365,22 +2500,22 @@
         <v>49</v>
       </c>
       <c r="C41" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="D41" s="2">
         <v>43511</v>
       </c>
       <c r="F41" t="s">
-        <v>254</v>
+        <v>299</v>
       </c>
       <c r="G41" t="s">
-        <v>258</v>
+        <v>303</v>
       </c>
       <c r="I41" t="s">
-        <v>262</v>
+        <v>307</v>
       </c>
       <c r="J41" t="s">
-        <v>302</v>
+        <v>347</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2391,16 +2526,16 @@
         <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="D42" s="2">
         <v>43511</v>
       </c>
       <c r="F42" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J42" t="s">
-        <v>303</v>
+        <v>348</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2411,16 +2546,16 @@
         <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="D43" s="2">
         <v>43511</v>
       </c>
       <c r="F43" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J43" t="s">
-        <v>304</v>
+        <v>349</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2431,16 +2566,16 @@
         <v>52</v>
       </c>
       <c r="C44" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="D44" s="2">
         <v>43511</v>
       </c>
       <c r="F44" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J44" t="s">
-        <v>305</v>
+        <v>350</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2451,16 +2586,16 @@
         <v>53</v>
       </c>
       <c r="C45" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="D45" s="2">
         <v>43511</v>
       </c>
       <c r="F45" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J45" t="s">
-        <v>306</v>
+        <v>351</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2471,16 +2606,16 @@
         <v>54</v>
       </c>
       <c r="C46" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
       <c r="D46" s="2">
         <v>43511</v>
       </c>
       <c r="F46" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J46" t="s">
-        <v>307</v>
+        <v>352</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2491,16 +2626,16 @@
         <v>55</v>
       </c>
       <c r="C47" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="D47" s="2">
         <v>43511</v>
       </c>
       <c r="F47" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J47" t="s">
-        <v>308</v>
+        <v>353</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2511,16 +2646,16 @@
         <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="D48" s="2">
         <v>43511</v>
       </c>
       <c r="F48" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J48" t="s">
-        <v>309</v>
+        <v>354</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2531,16 +2666,16 @@
         <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="D49" s="2">
         <v>43511</v>
       </c>
       <c r="F49" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J49" t="s">
-        <v>310</v>
+        <v>355</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2551,16 +2686,16 @@
         <v>58</v>
       </c>
       <c r="C50" t="s">
-        <v>180</v>
+        <v>202</v>
       </c>
       <c r="D50" s="2">
         <v>43511</v>
       </c>
       <c r="F50" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J50" t="s">
-        <v>311</v>
+        <v>356</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2571,16 +2706,16 @@
         <v>59</v>
       </c>
       <c r="C51" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
       <c r="D51" s="2">
         <v>43511</v>
       </c>
       <c r="F51" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J51" t="s">
-        <v>312</v>
+        <v>357</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2591,16 +2726,16 @@
         <v>60</v>
       </c>
       <c r="C52" t="s">
-        <v>182</v>
+        <v>204</v>
       </c>
       <c r="D52" s="2">
         <v>43511</v>
       </c>
       <c r="F52" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J52" t="s">
-        <v>313</v>
+        <v>358</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2611,16 +2746,16 @@
         <v>61</v>
       </c>
       <c r="C53" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="D53" s="2">
         <v>43511</v>
       </c>
       <c r="F53" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J53" t="s">
-        <v>314</v>
+        <v>359</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2631,16 +2766,16 @@
         <v>62</v>
       </c>
       <c r="C54" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="D54" s="2">
         <v>43511</v>
       </c>
       <c r="F54" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J54" t="s">
-        <v>315</v>
+        <v>360</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2651,16 +2786,16 @@
         <v>63</v>
       </c>
       <c r="C55" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
       <c r="D55" s="2">
         <v>43511</v>
       </c>
       <c r="F55" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J55" t="s">
-        <v>316</v>
+        <v>361</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2671,16 +2806,16 @@
         <v>64</v>
       </c>
       <c r="C56" t="s">
-        <v>186</v>
+        <v>208</v>
       </c>
       <c r="D56" s="2">
         <v>43511</v>
       </c>
       <c r="F56" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J56" t="s">
-        <v>317</v>
+        <v>362</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2691,16 +2826,16 @@
         <v>65</v>
       </c>
       <c r="C57" t="s">
-        <v>187</v>
+        <v>209</v>
       </c>
       <c r="D57" s="2">
         <v>43511</v>
       </c>
       <c r="F57" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J57" t="s">
-        <v>318</v>
+        <v>363</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2711,16 +2846,16 @@
         <v>66</v>
       </c>
       <c r="C58" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="D58" s="2">
         <v>43511</v>
       </c>
       <c r="F58" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J58" t="s">
-        <v>319</v>
+        <v>364</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2731,16 +2866,16 @@
         <v>67</v>
       </c>
       <c r="C59" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
       <c r="D59" s="2">
         <v>43511</v>
       </c>
       <c r="F59" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J59" t="s">
-        <v>320</v>
+        <v>365</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2751,16 +2886,16 @@
         <v>68</v>
       </c>
       <c r="C60" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="D60" s="2">
         <v>43511</v>
       </c>
       <c r="F60" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J60" t="s">
-        <v>321</v>
+        <v>366</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -2771,16 +2906,16 @@
         <v>69</v>
       </c>
       <c r="C61" t="s">
-        <v>191</v>
+        <v>213</v>
       </c>
       <c r="D61" s="2">
         <v>43511</v>
       </c>
       <c r="F61" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J61" t="s">
-        <v>322</v>
+        <v>367</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2791,16 +2926,16 @@
         <v>70</v>
       </c>
       <c r="C62" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="D62" s="2">
         <v>43511</v>
       </c>
       <c r="F62" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J62" t="s">
-        <v>323</v>
+        <v>368</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2811,16 +2946,16 @@
         <v>71</v>
       </c>
       <c r="C63" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="D63" s="2">
         <v>43511</v>
       </c>
       <c r="F63" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J63" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2831,16 +2966,16 @@
         <v>72</v>
       </c>
       <c r="C64" t="s">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="D64" s="2">
         <v>43511</v>
       </c>
       <c r="F64" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J64" t="s">
-        <v>325</v>
+        <v>370</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -2851,16 +2986,16 @@
         <v>73</v>
       </c>
       <c r="C65" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="D65" s="2">
         <v>43511</v>
       </c>
       <c r="F65" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J65" t="s">
-        <v>326</v>
+        <v>371</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -2871,16 +3006,16 @@
         <v>74</v>
       </c>
       <c r="C66" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
       <c r="D66" s="2">
         <v>43511</v>
       </c>
       <c r="F66" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J66" t="s">
-        <v>327</v>
+        <v>372</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2891,16 +3026,16 @@
         <v>75</v>
       </c>
       <c r="C67" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="D67" s="2">
         <v>43511</v>
       </c>
       <c r="F67" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J67" t="s">
-        <v>328</v>
+        <v>373</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -2911,16 +3046,16 @@
         <v>76</v>
       </c>
       <c r="C68" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="D68" s="2">
         <v>43511</v>
       </c>
       <c r="F68" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J68" t="s">
-        <v>329</v>
+        <v>374</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -2931,16 +3066,16 @@
         <v>77</v>
       </c>
       <c r="C69" t="s">
-        <v>199</v>
+        <v>221</v>
       </c>
       <c r="D69" s="2">
         <v>43512.02811368056</v>
       </c>
       <c r="F69" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J69" t="s">
-        <v>330</v>
+        <v>375</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -2951,16 +3086,16 @@
         <v>78</v>
       </c>
       <c r="C70" t="s">
-        <v>200</v>
+        <v>222</v>
       </c>
       <c r="D70" s="2">
         <v>43514.58475023148</v>
       </c>
       <c r="F70" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J70" t="s">
-        <v>331</v>
+        <v>376</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -2971,16 +3106,16 @@
         <v>79</v>
       </c>
       <c r="C71" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="D71" s="2">
         <v>43514.58475289352</v>
       </c>
       <c r="F71" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J71" t="s">
-        <v>332</v>
+        <v>377</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -2991,16 +3126,16 @@
         <v>80</v>
       </c>
       <c r="C72" t="s">
-        <v>202</v>
+        <v>224</v>
       </c>
       <c r="D72" s="2">
         <v>43514.58475601852</v>
       </c>
       <c r="F72" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J72" t="s">
-        <v>333</v>
+        <v>378</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -3011,16 +3146,16 @@
         <v>81</v>
       </c>
       <c r="C73" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="D73" s="2">
         <v>43514.58475809028</v>
       </c>
       <c r="F73" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J73" t="s">
-        <v>334</v>
+        <v>379</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -3031,16 +3166,16 @@
         <v>82</v>
       </c>
       <c r="C74" t="s">
-        <v>204</v>
+        <v>226</v>
       </c>
       <c r="D74" s="2">
         <v>43515.48238950231</v>
       </c>
       <c r="F74" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J74" t="s">
-        <v>335</v>
+        <v>380</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -3051,16 +3186,16 @@
         <v>83</v>
       </c>
       <c r="C75" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
       <c r="D75" s="2">
         <v>43515.73058116898</v>
       </c>
       <c r="F75" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J75" t="s">
-        <v>336</v>
+        <v>381</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -3071,16 +3206,16 @@
         <v>84</v>
       </c>
       <c r="C76" t="s">
-        <v>206</v>
+        <v>228</v>
       </c>
       <c r="D76" s="2">
         <v>43515.73058324074</v>
       </c>
       <c r="F76" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J76" t="s">
-        <v>337</v>
+        <v>382</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -3091,16 +3226,16 @@
         <v>85</v>
       </c>
       <c r="C77" t="s">
-        <v>207</v>
+        <v>229</v>
       </c>
       <c r="D77" s="2">
         <v>43516.4953059375</v>
       </c>
       <c r="F77" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J77" t="s">
-        <v>338</v>
+        <v>383</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -3111,16 +3246,16 @@
         <v>86</v>
       </c>
       <c r="C78" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="D78" s="2">
         <v>43518.61259846065</v>
       </c>
       <c r="F78" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J78" t="s">
-        <v>339</v>
+        <v>384</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -3131,16 +3266,16 @@
         <v>87</v>
       </c>
       <c r="C79" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="D79" s="2">
         <v>43521.6215687037</v>
       </c>
       <c r="F79" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J79" t="s">
-        <v>340</v>
+        <v>385</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -3151,16 +3286,16 @@
         <v>88</v>
       </c>
       <c r="C80" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="D80" s="2">
         <v>43521.6215702662</v>
       </c>
       <c r="F80" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J80" t="s">
-        <v>341</v>
+        <v>386</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -3171,16 +3306,16 @@
         <v>89</v>
       </c>
       <c r="C81" t="s">
-        <v>211</v>
+        <v>233</v>
       </c>
       <c r="D81" s="2">
         <v>43521.6215747338</v>
       </c>
       <c r="F81" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J81" t="s">
-        <v>342</v>
+        <v>387</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -3191,16 +3326,16 @@
         <v>90</v>
       </c>
       <c r="C82" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="D82" s="2">
         <v>43521.6215747338</v>
       </c>
       <c r="F82" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J82" t="s">
-        <v>343</v>
+        <v>388</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -3211,16 +3346,16 @@
         <v>91</v>
       </c>
       <c r="C83" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="D83" s="2">
         <v>43522.71610519676</v>
       </c>
       <c r="F83" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J83" t="s">
-        <v>344</v>
+        <v>389</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -3231,16 +3366,16 @@
         <v>92</v>
       </c>
       <c r="C84" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="D84" s="2">
         <v>43522.71610894676</v>
       </c>
       <c r="F84" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J84" t="s">
-        <v>345</v>
+        <v>390</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -3251,16 +3386,16 @@
         <v>93</v>
       </c>
       <c r="C85" t="s">
-        <v>215</v>
+        <v>237</v>
       </c>
       <c r="D85" s="2">
         <v>43523.38975456019</v>
       </c>
       <c r="F85" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J85" t="s">
-        <v>346</v>
+        <v>391</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -3271,16 +3406,16 @@
         <v>94</v>
       </c>
       <c r="C86" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="D86" s="2">
         <v>43524.45939690972</v>
       </c>
       <c r="F86" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J86" t="s">
-        <v>347</v>
+        <v>392</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -3291,16 +3426,16 @@
         <v>95</v>
       </c>
       <c r="C87" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="D87" s="2">
         <v>43524.45991893519</v>
       </c>
       <c r="F87" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J87" t="s">
-        <v>348</v>
+        <v>393</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -3311,16 +3446,16 @@
         <v>96</v>
       </c>
       <c r="C88" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="D88" s="2">
         <v>43524.45991893519</v>
       </c>
       <c r="F88" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J88" t="s">
-        <v>349</v>
+        <v>394</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -3331,687 +3466,1078 @@
         <v>97</v>
       </c>
       <c r="C89" t="s">
-        <v>219</v>
+        <v>241</v>
       </c>
       <c r="D89" s="2">
         <v>43524.45991893519</v>
       </c>
       <c r="F89" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J89" t="s">
-        <v>350</v>
+        <v>395</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B90" t="s">
         <v>98</v>
       </c>
       <c r="C90" t="s">
-        <v>220</v>
+        <v>242</v>
       </c>
       <c r="D90" s="2">
         <v>43529.37632800926</v>
       </c>
       <c r="F90" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J90" t="s">
-        <v>351</v>
+        <v>396</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B91" t="s">
         <v>99</v>
       </c>
       <c r="C91" t="s">
-        <v>221</v>
+        <v>243</v>
       </c>
       <c r="D91" s="2">
         <v>43529.37633297453</v>
       </c>
       <c r="F91" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J91" t="s">
-        <v>352</v>
+        <v>397</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B92" t="s">
         <v>100</v>
       </c>
       <c r="C92" t="s">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="D92" s="2">
         <v>43529.42497050926</v>
       </c>
       <c r="F92" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J92" t="s">
-        <v>353</v>
+        <v>398</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B93" t="s">
         <v>101</v>
       </c>
       <c r="C93" t="s">
-        <v>223</v>
+        <v>245</v>
       </c>
       <c r="D93" s="2">
         <v>43529.42497885416</v>
       </c>
       <c r="F93" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J93" t="s">
-        <v>354</v>
+        <v>399</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B94" t="s">
         <v>102</v>
       </c>
       <c r="C94" t="s">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="D94" s="2">
         <v>43529.48534415509</v>
       </c>
       <c r="F94" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J94" t="s">
-        <v>355</v>
+        <v>400</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B95" t="s">
         <v>103</v>
       </c>
       <c r="C95" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
       <c r="D95" s="2">
         <v>43529.74539105324</v>
       </c>
       <c r="F95" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J95" t="s">
-        <v>356</v>
+        <v>401</v>
       </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B96" t="s">
         <v>104</v>
       </c>
       <c r="C96" t="s">
-        <v>226</v>
+        <v>248</v>
       </c>
       <c r="D96" s="2">
         <v>43529.75238363426</v>
       </c>
       <c r="F96" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J96" t="s">
-        <v>357</v>
+        <v>402</v>
       </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B97" t="s">
         <v>105</v>
       </c>
       <c r="C97" t="s">
-        <v>227</v>
+        <v>249</v>
       </c>
       <c r="D97" s="2">
         <v>43529.7523853125</v>
       </c>
       <c r="F97" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J97" t="s">
-        <v>358</v>
+        <v>403</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B98" t="s">
         <v>106</v>
       </c>
       <c r="C98" t="s">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="D98" s="2">
         <v>43529.79556278935</v>
       </c>
       <c r="F98" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J98" t="s">
-        <v>359</v>
+        <v>404</v>
       </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B99" t="s">
         <v>107</v>
       </c>
       <c r="C99" t="s">
-        <v>229</v>
+        <v>251</v>
       </c>
       <c r="D99" s="2">
         <v>43530.39331518518</v>
       </c>
       <c r="F99" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J99" t="s">
-        <v>360</v>
+        <v>405</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B100" t="s">
         <v>108</v>
       </c>
       <c r="C100" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="D100" s="2">
         <v>43530.81668289352</v>
       </c>
       <c r="F100" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J100" t="s">
-        <v>361</v>
+        <v>406</v>
       </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B101" t="s">
         <v>109</v>
       </c>
       <c r="C101" t="s">
-        <v>231</v>
+        <v>253</v>
       </c>
       <c r="D101" s="2">
         <v>43530.81669511574</v>
       </c>
       <c r="F101" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J101" t="s">
-        <v>362</v>
+        <v>407</v>
       </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B102" t="s">
         <v>110</v>
       </c>
       <c r="C102" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="D102" s="2">
         <v>43532.40770633102</v>
       </c>
       <c r="F102" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J102" t="s">
-        <v>363</v>
+        <v>408</v>
       </c>
     </row>
     <row r="103" spans="1:10">
       <c r="A103">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B103" t="s">
         <v>111</v>
       </c>
       <c r="C103" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
       <c r="D103" s="2">
         <v>43532.40898523148</v>
       </c>
       <c r="F103" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J103" t="s">
-        <v>364</v>
+        <v>409</v>
       </c>
     </row>
     <row r="104" spans="1:10">
       <c r="A104">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B104" t="s">
         <v>112</v>
       </c>
       <c r="C104" t="s">
-        <v>234</v>
+        <v>256</v>
       </c>
       <c r="D104" s="2">
         <v>43532.59223354167</v>
       </c>
       <c r="F104" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J104" t="s">
-        <v>365</v>
+        <v>410</v>
       </c>
     </row>
     <row r="105" spans="1:10">
       <c r="A105">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B105" t="s">
         <v>113</v>
       </c>
       <c r="C105" t="s">
-        <v>235</v>
+        <v>257</v>
       </c>
       <c r="D105" s="2">
         <v>43535.35740248843</v>
       </c>
       <c r="F105" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J105" t="s">
-        <v>366</v>
+        <v>411</v>
       </c>
     </row>
     <row r="106" spans="1:10">
       <c r="A106">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B106" t="s">
         <v>114</v>
       </c>
       <c r="C106" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="D106" s="2">
         <v>43535.35740469908</v>
       </c>
       <c r="F106" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J106" t="s">
-        <v>367</v>
+        <v>412</v>
       </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B107" t="s">
         <v>115</v>
       </c>
       <c r="C107" t="s">
-        <v>237</v>
+        <v>259</v>
       </c>
       <c r="D107" s="2">
         <v>43535.35740587963</v>
       </c>
       <c r="F107" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J107" t="s">
-        <v>368</v>
+        <v>413</v>
       </c>
     </row>
     <row r="108" spans="1:10">
       <c r="A108">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B108" t="s">
         <v>116</v>
       </c>
       <c r="C108" t="s">
-        <v>238</v>
+        <v>260</v>
       </c>
       <c r="D108" s="2">
         <v>43535.35740699074</v>
       </c>
       <c r="F108" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J108" t="s">
-        <v>369</v>
+        <v>414</v>
       </c>
     </row>
     <row r="109" spans="1:10">
       <c r="A109">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B109" t="s">
         <v>117</v>
       </c>
       <c r="C109" t="s">
-        <v>239</v>
+        <v>261</v>
       </c>
       <c r="D109" s="2">
         <v>43535.35741133102</v>
       </c>
       <c r="F109" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J109" t="s">
-        <v>370</v>
+        <v>415</v>
       </c>
     </row>
     <row r="110" spans="1:10">
       <c r="A110">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B110" t="s">
         <v>118</v>
       </c>
       <c r="C110" t="s">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="D110" s="2">
         <v>43535.35741549769</v>
       </c>
       <c r="F110" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J110" t="s">
-        <v>371</v>
+        <v>416</v>
       </c>
     </row>
     <row r="111" spans="1:10">
       <c r="A111">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B111" t="s">
         <v>119</v>
       </c>
       <c r="C111" t="s">
-        <v>241</v>
+        <v>263</v>
       </c>
       <c r="D111" s="2">
         <v>43535.69687207176</v>
       </c>
       <c r="F111" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J111" t="s">
-        <v>372</v>
+        <v>417</v>
       </c>
     </row>
     <row r="112" spans="1:10">
       <c r="A112">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="B112" t="s">
         <v>120</v>
       </c>
       <c r="C112" t="s">
-        <v>242</v>
+        <v>264</v>
       </c>
       <c r="D112" s="2">
         <v>43535.69687763889</v>
       </c>
       <c r="F112" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J112" t="s">
-        <v>373</v>
+        <v>418</v>
       </c>
     </row>
     <row r="113" spans="1:10">
       <c r="A113">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B113" t="s">
         <v>121</v>
       </c>
       <c r="C113" t="s">
-        <v>243</v>
+        <v>265</v>
       </c>
       <c r="D113" s="2">
         <v>43535.72659671296</v>
       </c>
       <c r="F113" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J113" t="s">
-        <v>374</v>
+        <v>419</v>
       </c>
     </row>
     <row r="114" spans="1:10">
       <c r="A114">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B114" t="s">
         <v>122</v>
       </c>
       <c r="C114" t="s">
-        <v>244</v>
+        <v>266</v>
       </c>
       <c r="D114" s="2">
         <v>43537.40848363426</v>
       </c>
       <c r="F114" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J114" t="s">
-        <v>375</v>
+        <v>420</v>
       </c>
     </row>
     <row r="115" spans="1:10">
       <c r="A115">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B115" t="s">
         <v>123</v>
       </c>
       <c r="C115" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
       <c r="D115" s="2">
         <v>43538.43785037037</v>
       </c>
       <c r="F115" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J115" t="s">
-        <v>376</v>
+        <v>421</v>
       </c>
     </row>
     <row r="116" spans="1:10">
       <c r="A116">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B116" t="s">
         <v>124</v>
       </c>
       <c r="C116" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
       <c r="D116" s="2">
         <v>43538.45286440972</v>
       </c>
       <c r="F116" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J116" t="s">
-        <v>377</v>
+        <v>422</v>
       </c>
     </row>
     <row r="117" spans="1:10">
       <c r="A117">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="B117" t="s">
         <v>125</v>
       </c>
       <c r="C117" t="s">
-        <v>247</v>
+        <v>269</v>
       </c>
       <c r="D117" s="2">
         <v>43539.3654228588</v>
       </c>
       <c r="F117" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J117" t="s">
-        <v>378</v>
+        <v>423</v>
       </c>
     </row>
     <row r="118" spans="1:10">
       <c r="A118">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B118" t="s">
         <v>126</v>
       </c>
       <c r="C118" t="s">
-        <v>248</v>
+        <v>270</v>
       </c>
       <c r="D118" s="2">
         <v>43542.56313657408</v>
       </c>
       <c r="F118" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J118" t="s">
-        <v>379</v>
+        <v>424</v>
       </c>
     </row>
     <row r="119" spans="1:10">
       <c r="A119">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B119" t="s">
         <v>127</v>
       </c>
       <c r="C119" t="s">
-        <v>249</v>
+        <v>271</v>
       </c>
       <c r="D119" s="2">
         <v>43542.56314506944</v>
       </c>
       <c r="F119" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J119" t="s">
-        <v>380</v>
+        <v>425</v>
       </c>
     </row>
     <row r="120" spans="1:10">
       <c r="A120">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="B120" t="s">
         <v>128</v>
       </c>
       <c r="C120" t="s">
-        <v>250</v>
+        <v>272</v>
       </c>
       <c r="D120" s="2">
         <v>43542.56314643518</v>
       </c>
       <c r="F120" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="J120" t="s">
-        <v>381</v>
+        <v>426</v>
       </c>
     </row>
     <row r="121" spans="1:10">
       <c r="A121">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B121" t="s">
         <v>129</v>
       </c>
       <c r="C121" t="s">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="D121" s="2">
-        <v>43543.55330482867</v>
+        <v>43543.89551372685</v>
       </c>
       <c r="F121" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
     </row>
     <row r="122" spans="1:10">
       <c r="A122">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B122" t="s">
         <v>130</v>
       </c>
       <c r="C122" t="s">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="D122" s="2">
-        <v>43543.55330563703</v>
+        <v>43543.89551444445</v>
       </c>
       <c r="F122" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
     </row>
     <row r="123" spans="1:10">
       <c r="A123">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B123" t="s">
         <v>131</v>
       </c>
       <c r="C123" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
       <c r="D123" s="2">
-        <v>43543.55330700071</v>
+        <v>43543.89551589121</v>
       </c>
       <c r="F123" t="s">
-        <v>255</v>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
+      <c r="A124">
+        <v>0</v>
+      </c>
+      <c r="B124" t="s">
+        <v>132</v>
+      </c>
+      <c r="C124" t="s">
+        <v>276</v>
+      </c>
+      <c r="D124" s="2">
+        <v>43543.89551679398</v>
+      </c>
+      <c r="F124" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
+      <c r="A125">
+        <v>0</v>
+      </c>
+      <c r="B125" t="s">
+        <v>133</v>
+      </c>
+      <c r="C125" t="s">
+        <v>277</v>
+      </c>
+      <c r="D125" s="2">
+        <v>43544.75425299769</v>
+      </c>
+      <c r="F125" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
+      <c r="A126">
+        <v>0</v>
+      </c>
+      <c r="B126" t="s">
+        <v>134</v>
+      </c>
+      <c r="C126" t="s">
+        <v>278</v>
+      </c>
+      <c r="D126" s="2">
+        <v>43544.75426621528</v>
+      </c>
+      <c r="F126" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
+      <c r="A127">
+        <v>0</v>
+      </c>
+      <c r="B127" t="s">
+        <v>135</v>
+      </c>
+      <c r="C127" t="s">
+        <v>279</v>
+      </c>
+      <c r="D127" s="2">
+        <v>43545.75100377315</v>
+      </c>
+      <c r="F127" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
+      <c r="A128">
+        <v>0</v>
+      </c>
+      <c r="B128" t="s">
+        <v>136</v>
+      </c>
+      <c r="C128" t="s">
+        <v>280</v>
+      </c>
+      <c r="D128" s="2">
+        <v>43545.75100574074</v>
+      </c>
+      <c r="F128" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129">
+        <v>0</v>
+      </c>
+      <c r="B129" t="s">
+        <v>137</v>
+      </c>
+      <c r="C129" t="s">
+        <v>281</v>
+      </c>
+      <c r="D129" s="2">
+        <v>43551.67338550926</v>
+      </c>
+      <c r="F129" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130">
+        <v>0</v>
+      </c>
+      <c r="B130" t="s">
+        <v>138</v>
+      </c>
+      <c r="C130" t="s">
+        <v>282</v>
+      </c>
+      <c r="D130" s="2">
+        <v>43551.67353653935</v>
+      </c>
+      <c r="F130" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131">
+        <v>0</v>
+      </c>
+      <c r="B131" t="s">
+        <v>139</v>
+      </c>
+      <c r="C131" t="s">
+        <v>283</v>
+      </c>
+      <c r="D131" s="2">
+        <v>43551.67353653935</v>
+      </c>
+      <c r="F131" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132">
+        <v>0</v>
+      </c>
+      <c r="B132" t="s">
+        <v>97</v>
+      </c>
+      <c r="C132" t="s">
+        <v>284</v>
+      </c>
+      <c r="D132" s="2">
+        <v>43551.67353653935</v>
+      </c>
+      <c r="F132" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133">
+        <v>0</v>
+      </c>
+      <c r="B133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C133" t="s">
+        <v>285</v>
+      </c>
+      <c r="D133" s="2">
+        <v>43551.6936352199</v>
+      </c>
+      <c r="F133" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134">
+        <v>0</v>
+      </c>
+      <c r="B134" t="s">
+        <v>141</v>
+      </c>
+      <c r="C134" t="s">
+        <v>286</v>
+      </c>
+      <c r="D134" s="2">
+        <v>43553.46505314815</v>
+      </c>
+      <c r="F134" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135">
+        <v>0</v>
+      </c>
+      <c r="B135" t="s">
+        <v>142</v>
+      </c>
+      <c r="C135" t="s">
+        <v>287</v>
+      </c>
+      <c r="D135" s="2">
+        <v>43553.46505376157</v>
+      </c>
+      <c r="F135" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136">
+        <v>1</v>
+      </c>
+      <c r="B136" t="s">
+        <v>143</v>
+      </c>
+      <c r="C136" t="s">
+        <v>288</v>
+      </c>
+      <c r="D136" s="2">
+        <v>43556.43366586805</v>
+      </c>
+      <c r="F136" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137">
+        <v>2</v>
+      </c>
+      <c r="B137" t="s">
+        <v>144</v>
+      </c>
+      <c r="C137" t="s">
+        <v>289</v>
+      </c>
+      <c r="D137" s="2">
+        <v>43556.4336666551</v>
+      </c>
+      <c r="F137" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138">
+        <v>3</v>
+      </c>
+      <c r="B138" t="s">
+        <v>145</v>
+      </c>
+      <c r="C138" t="s">
+        <v>290</v>
+      </c>
+      <c r="D138" s="2">
+        <v>43556.49071166667</v>
+      </c>
+      <c r="F138" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139">
+        <v>4</v>
+      </c>
+      <c r="B139" t="s">
+        <v>146</v>
+      </c>
+      <c r="C139" t="s">
+        <v>291</v>
+      </c>
+      <c r="D139" s="2">
+        <v>43560.59194121528</v>
+      </c>
+      <c r="F139" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140">
+        <v>5</v>
+      </c>
+      <c r="B140" t="s">
+        <v>147</v>
+      </c>
+      <c r="C140" t="s">
+        <v>292</v>
+      </c>
+      <c r="D140" s="2">
+        <v>43560.59194184028</v>
+      </c>
+      <c r="F140" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141">
+        <v>6</v>
+      </c>
+      <c r="B141" t="s">
+        <v>148</v>
+      </c>
+      <c r="C141" t="s">
+        <v>293</v>
+      </c>
+      <c r="D141" s="2">
+        <v>43560.59194243055</v>
+      </c>
+      <c r="F141" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142">
+        <v>7</v>
+      </c>
+      <c r="B142" t="s">
+        <v>149</v>
+      </c>
+      <c r="C142" t="s">
+        <v>294</v>
+      </c>
+      <c r="D142" s="2">
+        <v>43560.59194300926</v>
+      </c>
+      <c r="F142" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143">
+        <v>8</v>
+      </c>
+      <c r="B143" t="s">
+        <v>150</v>
+      </c>
+      <c r="C143" t="s">
+        <v>295</v>
+      </c>
+      <c r="D143" s="2">
+        <v>43560.67661109954</v>
+      </c>
+      <c r="F143" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144">
+        <v>9</v>
+      </c>
+      <c r="B144" t="s">
+        <v>151</v>
+      </c>
+      <c r="C144" t="s">
+        <v>296</v>
+      </c>
+      <c r="D144" s="2">
+        <v>43563.95673027778</v>
+      </c>
+      <c r="F144" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145">
+        <v>10</v>
+      </c>
+      <c r="B145" t="s">
+        <v>152</v>
+      </c>
+      <c r="C145" t="s">
+        <v>297</v>
+      </c>
+      <c r="D145" s="2">
+        <v>43563.95673082176</v>
+      </c>
+      <c r="F145" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146">
+        <v>11</v>
+      </c>
+      <c r="B146" t="s">
+        <v>153</v>
+      </c>
+      <c r="C146" t="s">
+        <v>298</v>
+      </c>
+      <c r="D146" s="2">
+        <v>43563.95673144676</v>
+      </c>
+      <c r="F146" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add exception catch for get_nodin index error and return placeholder nodin number. It happen when there is invalid character in the email subject
</commit_message>
<xml_diff>
--- a/New Products Assmt.xlsx
+++ b/New Products Assmt.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wahyu\PT Telekomunikasi Selular\muhammad_f_rais - POSTPAID REVAS onedrive\New Products Assurance\script\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_CF969CDF7ED96CE42849BBAFF95EF0F5502D08BD" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{85DF0075-346E-4C2B-97C4-704FE7EEFDD5}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1300,11 +1306,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1368,6 +1374,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1414,7 +1428,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1446,9 +1460,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1480,6 +1512,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1655,14 +1705,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J146"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="A147" sqref="A147:F150"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1694,7 +1746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1720,7 +1772,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1746,7 +1798,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1766,7 +1818,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1786,7 +1838,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -1809,7 +1861,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1832,7 +1884,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1852,7 +1904,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -1872,7 +1924,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1892,7 +1944,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1912,7 +1964,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
@@ -1932,7 +1984,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
@@ -1952,7 +2004,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -1972,7 +2024,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1992,7 +2044,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
@@ -2012,7 +2064,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
@@ -2032,7 +2084,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -2052,7 +2104,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -2072,7 +2124,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -2092,7 +2144,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -2112,7 +2164,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0</v>
       </c>
@@ -2132,7 +2184,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2152,7 +2204,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0</v>
       </c>
@@ -2172,7 +2224,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0</v>
       </c>
@@ -2192,7 +2244,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
@@ -2212,7 +2264,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
@@ -2232,7 +2284,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0</v>
       </c>
@@ -2252,7 +2304,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0</v>
       </c>
@@ -2272,7 +2324,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0</v>
       </c>
@@ -2292,7 +2344,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -2312,7 +2364,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0</v>
       </c>
@@ -2332,7 +2384,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0</v>
       </c>
@@ -2352,7 +2404,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>0</v>
       </c>
@@ -2372,7 +2424,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>0</v>
       </c>
@@ -2392,7 +2444,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>0</v>
       </c>
@@ -2412,7 +2464,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>0</v>
       </c>
@@ -2432,7 +2484,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>0</v>
       </c>
@@ -2452,7 +2504,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0</v>
       </c>
@@ -2472,7 +2524,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>0</v>
       </c>
@@ -2492,7 +2544,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0</v>
       </c>
@@ -2518,7 +2570,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>0</v>
       </c>
@@ -2538,7 +2590,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>0</v>
       </c>
@@ -2558,7 +2610,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>0</v>
       </c>
@@ -2578,7 +2630,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>0</v>
       </c>
@@ -2598,7 +2650,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>0</v>
       </c>
@@ -2618,7 +2670,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>0</v>
       </c>
@@ -2638,7 +2690,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>0</v>
       </c>
@@ -2658,7 +2710,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>0</v>
       </c>
@@ -2678,7 +2730,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>0</v>
       </c>
@@ -2698,7 +2750,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>0</v>
       </c>
@@ -2718,7 +2770,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>0</v>
       </c>
@@ -2738,7 +2790,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>0</v>
       </c>
@@ -2758,7 +2810,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>0</v>
       </c>
@@ -2778,7 +2830,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>0</v>
       </c>
@@ -2798,7 +2850,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>0</v>
       </c>
@@ -2818,7 +2870,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>0</v>
       </c>
@@ -2838,7 +2890,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>0</v>
       </c>
@@ -2858,7 +2910,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>0</v>
       </c>
@@ -2878,7 +2930,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>0</v>
       </c>
@@ -2898,7 +2950,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>0</v>
       </c>
@@ -2918,7 +2970,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>0</v>
       </c>
@@ -2938,7 +2990,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>0</v>
       </c>
@@ -2958,7 +3010,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>0</v>
       </c>
@@ -2978,7 +3030,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>0</v>
       </c>
@@ -2998,7 +3050,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>0</v>
       </c>
@@ -3018,7 +3070,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>0</v>
       </c>
@@ -3038,7 +3090,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>0</v>
       </c>
@@ -3058,7 +3110,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>0</v>
       </c>
@@ -3069,7 +3121,7 @@
         <v>221</v>
       </c>
       <c r="D69" s="2">
-        <v>43512.02811368056</v>
+        <v>43512.028113680557</v>
       </c>
       <c r="F69" t="s">
         <v>300</v>
@@ -3078,7 +3130,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>0</v>
       </c>
@@ -3089,7 +3141,7 @@
         <v>222</v>
       </c>
       <c r="D70" s="2">
-        <v>43514.58475023148</v>
+        <v>43514.584750231479</v>
       </c>
       <c r="F70" t="s">
         <v>300</v>
@@ -3098,7 +3150,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>0</v>
       </c>
@@ -3109,7 +3161,7 @@
         <v>223</v>
       </c>
       <c r="D71" s="2">
-        <v>43514.58475289352</v>
+        <v>43514.584752893519</v>
       </c>
       <c r="F71" t="s">
         <v>300</v>
@@ -3118,7 +3170,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>0</v>
       </c>
@@ -3129,7 +3181,7 @@
         <v>224</v>
       </c>
       <c r="D72" s="2">
-        <v>43514.58475601852</v>
+        <v>43514.584756018521</v>
       </c>
       <c r="F72" t="s">
         <v>300</v>
@@ -3138,7 +3190,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>0</v>
       </c>
@@ -3149,7 +3201,7 @@
         <v>225</v>
       </c>
       <c r="D73" s="2">
-        <v>43514.58475809028</v>
+        <v>43514.584758090277</v>
       </c>
       <c r="F73" t="s">
         <v>300</v>
@@ -3158,7 +3210,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>0</v>
       </c>
@@ -3169,7 +3221,7 @@
         <v>226</v>
       </c>
       <c r="D74" s="2">
-        <v>43515.48238950231</v>
+        <v>43515.482389502307</v>
       </c>
       <c r="F74" t="s">
         <v>300</v>
@@ -3178,7 +3230,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>0</v>
       </c>
@@ -3198,7 +3250,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>0</v>
       </c>
@@ -3209,7 +3261,7 @@
         <v>228</v>
       </c>
       <c r="D76" s="2">
-        <v>43515.73058324074</v>
+        <v>43515.730583240736</v>
       </c>
       <c r="F76" t="s">
         <v>300</v>
@@ -3218,7 +3270,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>0</v>
       </c>
@@ -3229,7 +3281,7 @@
         <v>229</v>
       </c>
       <c r="D77" s="2">
-        <v>43516.4953059375</v>
+        <v>43516.495305937497</v>
       </c>
       <c r="F77" t="s">
         <v>300</v>
@@ -3238,7 +3290,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>0</v>
       </c>
@@ -3249,7 +3301,7 @@
         <v>230</v>
       </c>
       <c r="D78" s="2">
-        <v>43518.61259846065</v>
+        <v>43518.612598460648</v>
       </c>
       <c r="F78" t="s">
         <v>300</v>
@@ -3258,7 +3310,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>0</v>
       </c>
@@ -3269,7 +3321,7 @@
         <v>231</v>
       </c>
       <c r="D79" s="2">
-        <v>43521.6215687037</v>
+        <v>43521.621568703697</v>
       </c>
       <c r="F79" t="s">
         <v>300</v>
@@ -3278,7 +3330,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>0</v>
       </c>
@@ -3289,7 +3341,7 @@
         <v>232</v>
       </c>
       <c r="D80" s="2">
-        <v>43521.6215702662</v>
+        <v>43521.621570266201</v>
       </c>
       <c r="F80" t="s">
         <v>300</v>
@@ -3298,7 +3350,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>0</v>
       </c>
@@ -3309,7 +3361,7 @@
         <v>233</v>
       </c>
       <c r="D81" s="2">
-        <v>43521.6215747338</v>
+        <v>43521.621574733799</v>
       </c>
       <c r="F81" t="s">
         <v>300</v>
@@ -3318,7 +3370,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>0</v>
       </c>
@@ -3329,7 +3381,7 @@
         <v>234</v>
       </c>
       <c r="D82" s="2">
-        <v>43521.6215747338</v>
+        <v>43521.621574733799</v>
       </c>
       <c r="F82" t="s">
         <v>300</v>
@@ -3338,7 +3390,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>0</v>
       </c>
@@ -3349,7 +3401,7 @@
         <v>235</v>
       </c>
       <c r="D83" s="2">
-        <v>43522.71610519676</v>
+        <v>43522.716105196763</v>
       </c>
       <c r="F83" t="s">
         <v>300</v>
@@ -3358,7 +3410,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>0</v>
       </c>
@@ -3369,7 +3421,7 @@
         <v>236</v>
       </c>
       <c r="D84" s="2">
-        <v>43522.71610894676</v>
+        <v>43522.716108946763</v>
       </c>
       <c r="F84" t="s">
         <v>300</v>
@@ -3378,7 +3430,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>0</v>
       </c>
@@ -3389,7 +3441,7 @@
         <v>237</v>
       </c>
       <c r="D85" s="2">
-        <v>43523.38975456019</v>
+        <v>43523.389754560187</v>
       </c>
       <c r="F85" t="s">
         <v>300</v>
@@ -3398,7 +3450,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>0</v>
       </c>
@@ -3409,7 +3461,7 @@
         <v>238</v>
       </c>
       <c r="D86" s="2">
-        <v>43524.45939690972</v>
+        <v>43524.459396909719</v>
       </c>
       <c r="F86" t="s">
         <v>300</v>
@@ -3418,7 +3470,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>0</v>
       </c>
@@ -3429,7 +3481,7 @@
         <v>239</v>
       </c>
       <c r="D87" s="2">
-        <v>43524.45991893519</v>
+        <v>43524.459918935187</v>
       </c>
       <c r="F87" t="s">
         <v>300</v>
@@ -3438,7 +3490,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>0</v>
       </c>
@@ -3449,7 +3501,7 @@
         <v>240</v>
       </c>
       <c r="D88" s="2">
-        <v>43524.45991893519</v>
+        <v>43524.459918935187</v>
       </c>
       <c r="F88" t="s">
         <v>300</v>
@@ -3458,7 +3510,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>0</v>
       </c>
@@ -3469,7 +3521,7 @@
         <v>241</v>
       </c>
       <c r="D89" s="2">
-        <v>43524.45991893519</v>
+        <v>43524.459918935187</v>
       </c>
       <c r="F89" t="s">
         <v>300</v>
@@ -3478,7 +3530,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>0</v>
       </c>
@@ -3489,7 +3541,7 @@
         <v>242</v>
       </c>
       <c r="D90" s="2">
-        <v>43529.37632800926</v>
+        <v>43529.376328009261</v>
       </c>
       <c r="F90" t="s">
         <v>300</v>
@@ -3498,7 +3550,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>0</v>
       </c>
@@ -3509,7 +3561,7 @@
         <v>243</v>
       </c>
       <c r="D91" s="2">
-        <v>43529.37633297453</v>
+        <v>43529.376332974527</v>
       </c>
       <c r="F91" t="s">
         <v>300</v>
@@ -3518,7 +3570,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>0</v>
       </c>
@@ -3529,7 +3581,7 @@
         <v>244</v>
       </c>
       <c r="D92" s="2">
-        <v>43529.42497050926</v>
+        <v>43529.424970509259</v>
       </c>
       <c r="F92" t="s">
         <v>300</v>
@@ -3538,7 +3590,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>0</v>
       </c>
@@ -3549,7 +3601,7 @@
         <v>245</v>
       </c>
       <c r="D93" s="2">
-        <v>43529.42497885416</v>
+        <v>43529.424978854157</v>
       </c>
       <c r="F93" t="s">
         <v>300</v>
@@ -3558,7 +3610,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>0</v>
       </c>
@@ -3569,7 +3621,7 @@
         <v>246</v>
       </c>
       <c r="D94" s="2">
-        <v>43529.48534415509</v>
+        <v>43529.485344155088</v>
       </c>
       <c r="F94" t="s">
         <v>300</v>
@@ -3578,7 +3630,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>0</v>
       </c>
@@ -3589,7 +3641,7 @@
         <v>247</v>
       </c>
       <c r="D95" s="2">
-        <v>43529.74539105324</v>
+        <v>43529.745391053242</v>
       </c>
       <c r="F95" t="s">
         <v>300</v>
@@ -3598,7 +3650,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>0</v>
       </c>
@@ -3609,7 +3661,7 @@
         <v>248</v>
       </c>
       <c r="D96" s="2">
-        <v>43529.75238363426</v>
+        <v>43529.752383634259</v>
       </c>
       <c r="F96" t="s">
         <v>300</v>
@@ -3618,7 +3670,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>0</v>
       </c>
@@ -3629,7 +3681,7 @@
         <v>249</v>
       </c>
       <c r="D97" s="2">
-        <v>43529.7523853125</v>
+        <v>43529.752385312502</v>
       </c>
       <c r="F97" t="s">
         <v>300</v>
@@ -3638,7 +3690,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>0</v>
       </c>
@@ -3649,7 +3701,7 @@
         <v>250</v>
       </c>
       <c r="D98" s="2">
-        <v>43529.79556278935</v>
+        <v>43529.795562789353</v>
       </c>
       <c r="F98" t="s">
         <v>300</v>
@@ -3658,7 +3710,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>0</v>
       </c>
@@ -3669,7 +3721,7 @@
         <v>251</v>
       </c>
       <c r="D99" s="2">
-        <v>43530.39331518518</v>
+        <v>43530.393315185182</v>
       </c>
       <c r="F99" t="s">
         <v>300</v>
@@ -3678,7 +3730,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>0</v>
       </c>
@@ -3689,7 +3741,7 @@
         <v>252</v>
       </c>
       <c r="D100" s="2">
-        <v>43530.81668289352</v>
+        <v>43530.816682893521</v>
       </c>
       <c r="F100" t="s">
         <v>300</v>
@@ -3698,7 +3750,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>0</v>
       </c>
@@ -3718,7 +3770,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>0</v>
       </c>
@@ -3729,7 +3781,7 @@
         <v>254</v>
       </c>
       <c r="D102" s="2">
-        <v>43532.40770633102</v>
+        <v>43532.407706331018</v>
       </c>
       <c r="F102" t="s">
         <v>300</v>
@@ -3738,7 +3790,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>0</v>
       </c>
@@ -3749,7 +3801,7 @@
         <v>255</v>
       </c>
       <c r="D103" s="2">
-        <v>43532.40898523148</v>
+        <v>43532.408985231479</v>
       </c>
       <c r="F103" t="s">
         <v>300</v>
@@ -3758,7 +3810,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>0</v>
       </c>
@@ -3769,7 +3821,7 @@
         <v>256</v>
       </c>
       <c r="D104" s="2">
-        <v>43532.59223354167</v>
+        <v>43532.592233541669</v>
       </c>
       <c r="F104" t="s">
         <v>300</v>
@@ -3778,7 +3830,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>0</v>
       </c>
@@ -3789,7 +3841,7 @@
         <v>257</v>
       </c>
       <c r="D105" s="2">
-        <v>43535.35740248843</v>
+        <v>43535.357402488429</v>
       </c>
       <c r="F105" t="s">
         <v>300</v>
@@ -3798,7 +3850,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>0</v>
       </c>
@@ -3809,7 +3861,7 @@
         <v>258</v>
       </c>
       <c r="D106" s="2">
-        <v>43535.35740469908</v>
+        <v>43535.357404699083</v>
       </c>
       <c r="F106" t="s">
         <v>300</v>
@@ -3818,7 +3870,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>0</v>
       </c>
@@ -3829,7 +3881,7 @@
         <v>259</v>
       </c>
       <c r="D107" s="2">
-        <v>43535.35740587963</v>
+        <v>43535.357405879629</v>
       </c>
       <c r="F107" t="s">
         <v>300</v>
@@ -3838,7 +3890,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>0</v>
       </c>
@@ -3849,7 +3901,7 @@
         <v>260</v>
       </c>
       <c r="D108" s="2">
-        <v>43535.35740699074</v>
+        <v>43535.357406990741</v>
       </c>
       <c r="F108" t="s">
         <v>300</v>
@@ -3858,7 +3910,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>0</v>
       </c>
@@ -3869,7 +3921,7 @@
         <v>261</v>
       </c>
       <c r="D109" s="2">
-        <v>43535.35741133102</v>
+        <v>43535.357411331017</v>
       </c>
       <c r="F109" t="s">
         <v>300</v>
@@ -3878,7 +3930,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>0</v>
       </c>
@@ -3889,7 +3941,7 @@
         <v>262</v>
       </c>
       <c r="D110" s="2">
-        <v>43535.35741549769</v>
+        <v>43535.357415497689</v>
       </c>
       <c r="F110" t="s">
         <v>300</v>
@@ -3898,7 +3950,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>0</v>
       </c>
@@ -3909,7 +3961,7 @@
         <v>263</v>
       </c>
       <c r="D111" s="2">
-        <v>43535.69687207176</v>
+        <v>43535.696872071763</v>
       </c>
       <c r="F111" t="s">
         <v>300</v>
@@ -3918,7 +3970,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>0</v>
       </c>
@@ -3929,7 +3981,7 @@
         <v>264</v>
       </c>
       <c r="D112" s="2">
-        <v>43535.69687763889</v>
+        <v>43535.696877638889</v>
       </c>
       <c r="F112" t="s">
         <v>300</v>
@@ -3938,7 +3990,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>0</v>
       </c>
@@ -3949,7 +4001,7 @@
         <v>265</v>
       </c>
       <c r="D113" s="2">
-        <v>43535.72659671296</v>
+        <v>43535.726596712957</v>
       </c>
       <c r="F113" t="s">
         <v>300</v>
@@ -3958,7 +4010,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>0</v>
       </c>
@@ -3969,7 +4021,7 @@
         <v>266</v>
       </c>
       <c r="D114" s="2">
-        <v>43537.40848363426</v>
+        <v>43537.408483634259</v>
       </c>
       <c r="F114" t="s">
         <v>300</v>
@@ -3978,7 +4030,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>0</v>
       </c>
@@ -3998,7 +4050,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>0</v>
       </c>
@@ -4009,7 +4061,7 @@
         <v>268</v>
       </c>
       <c r="D116" s="2">
-        <v>43538.45286440972</v>
+        <v>43538.452864409723</v>
       </c>
       <c r="F116" t="s">
         <v>300</v>
@@ -4018,7 +4070,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>0</v>
       </c>
@@ -4029,7 +4081,7 @@
         <v>269</v>
       </c>
       <c r="D117" s="2">
-        <v>43539.3654228588</v>
+        <v>43539.365422858798</v>
       </c>
       <c r="F117" t="s">
         <v>300</v>
@@ -4038,7 +4090,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>0</v>
       </c>
@@ -4049,7 +4101,7 @@
         <v>270</v>
       </c>
       <c r="D118" s="2">
-        <v>43542.56313657408</v>
+        <v>43542.563136574077</v>
       </c>
       <c r="F118" t="s">
         <v>300</v>
@@ -4058,7 +4110,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>0</v>
       </c>
@@ -4069,7 +4121,7 @@
         <v>271</v>
       </c>
       <c r="D119" s="2">
-        <v>43542.56314506944</v>
+        <v>43542.563145069442</v>
       </c>
       <c r="F119" t="s">
         <v>300</v>
@@ -4078,7 +4130,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>0</v>
       </c>
@@ -4089,7 +4141,7 @@
         <v>272</v>
       </c>
       <c r="D120" s="2">
-        <v>43542.56314643518</v>
+        <v>43542.563146435183</v>
       </c>
       <c r="F120" t="s">
         <v>300</v>
@@ -4098,7 +4150,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>0</v>
       </c>
@@ -4109,13 +4161,13 @@
         <v>273</v>
       </c>
       <c r="D121" s="2">
-        <v>43543.89551372685</v>
+        <v>43543.895513726849</v>
       </c>
       <c r="F121" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>0</v>
       </c>
@@ -4126,13 +4178,13 @@
         <v>274</v>
       </c>
       <c r="D122" s="2">
-        <v>43543.89551444445</v>
+        <v>43543.895514444448</v>
       </c>
       <c r="F122" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>0</v>
       </c>
@@ -4143,13 +4195,13 @@
         <v>275</v>
       </c>
       <c r="D123" s="2">
-        <v>43543.89551589121</v>
+        <v>43543.895515891207</v>
       </c>
       <c r="F123" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>0</v>
       </c>
@@ -4160,13 +4212,13 @@
         <v>276</v>
       </c>
       <c r="D124" s="2">
-        <v>43543.89551679398</v>
+        <v>43543.895516793978</v>
       </c>
       <c r="F124" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>0</v>
       </c>
@@ -4177,13 +4229,13 @@
         <v>277</v>
       </c>
       <c r="D125" s="2">
-        <v>43544.75425299769</v>
+        <v>43544.754252997693</v>
       </c>
       <c r="F125" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>0</v>
       </c>
@@ -4194,13 +4246,13 @@
         <v>278</v>
       </c>
       <c r="D126" s="2">
-        <v>43544.75426621528</v>
+        <v>43544.754266215277</v>
       </c>
       <c r="F126" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>0</v>
       </c>
@@ -4211,13 +4263,13 @@
         <v>279</v>
       </c>
       <c r="D127" s="2">
-        <v>43545.75100377315</v>
+        <v>43545.751003773148</v>
       </c>
       <c r="F127" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>0</v>
       </c>
@@ -4228,13 +4280,13 @@
         <v>280</v>
       </c>
       <c r="D128" s="2">
-        <v>43545.75100574074</v>
+        <v>43545.751005740742</v>
       </c>
       <c r="F128" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>0</v>
       </c>
@@ -4245,13 +4297,13 @@
         <v>281</v>
       </c>
       <c r="D129" s="2">
-        <v>43551.67338550926</v>
+        <v>43551.673385509261</v>
       </c>
       <c r="F129" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>0</v>
       </c>
@@ -4262,13 +4314,13 @@
         <v>282</v>
       </c>
       <c r="D130" s="2">
-        <v>43551.67353653935</v>
+        <v>43551.673536539347</v>
       </c>
       <c r="F130" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>0</v>
       </c>
@@ -4279,13 +4331,13 @@
         <v>283</v>
       </c>
       <c r="D131" s="2">
-        <v>43551.67353653935</v>
+        <v>43551.673536539347</v>
       </c>
       <c r="F131" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>0</v>
       </c>
@@ -4296,13 +4348,13 @@
         <v>284</v>
       </c>
       <c r="D132" s="2">
-        <v>43551.67353653935</v>
+        <v>43551.673536539347</v>
       </c>
       <c r="F132" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>0</v>
       </c>
@@ -4313,13 +4365,13 @@
         <v>285</v>
       </c>
       <c r="D133" s="2">
-        <v>43551.6936352199</v>
+        <v>43551.693635219897</v>
       </c>
       <c r="F133" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>0</v>
       </c>
@@ -4330,13 +4382,13 @@
         <v>286</v>
       </c>
       <c r="D134" s="2">
-        <v>43553.46505314815</v>
+        <v>43553.465053148153</v>
       </c>
       <c r="F134" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>0</v>
       </c>
@@ -4347,13 +4399,13 @@
         <v>287</v>
       </c>
       <c r="D135" s="2">
-        <v>43553.46505376157</v>
+        <v>43553.465053761567</v>
       </c>
       <c r="F135" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>1</v>
       </c>
@@ -4364,13 +4416,13 @@
         <v>288</v>
       </c>
       <c r="D136" s="2">
-        <v>43556.43366586805</v>
+        <v>43556.433665868048</v>
       </c>
       <c r="F136" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>2</v>
       </c>
@@ -4381,13 +4433,13 @@
         <v>289</v>
       </c>
       <c r="D137" s="2">
-        <v>43556.4336666551</v>
+        <v>43556.433666655103</v>
       </c>
       <c r="F137" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>3</v>
       </c>
@@ -4398,13 +4450,13 @@
         <v>290</v>
       </c>
       <c r="D138" s="2">
-        <v>43556.49071166667</v>
+        <v>43556.490711666673</v>
       </c>
       <c r="F138" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>4</v>
       </c>
@@ -4421,7 +4473,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>5</v>
       </c>
@@ -4432,13 +4484,13 @@
         <v>292</v>
       </c>
       <c r="D140" s="2">
-        <v>43560.59194184028</v>
+        <v>43560.591941840277</v>
       </c>
       <c r="F140" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>6</v>
       </c>
@@ -4449,13 +4501,13 @@
         <v>293</v>
       </c>
       <c r="D141" s="2">
-        <v>43560.59194243055</v>
+        <v>43560.591942430547</v>
       </c>
       <c r="F141" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>7</v>
       </c>
@@ -4466,13 +4518,13 @@
         <v>294</v>
       </c>
       <c r="D142" s="2">
-        <v>43560.59194300926</v>
+        <v>43560.591943009262</v>
       </c>
       <c r="F142" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>8</v>
       </c>
@@ -4483,13 +4535,13 @@
         <v>295</v>
       </c>
       <c r="D143" s="2">
-        <v>43560.67661109954</v>
+        <v>43560.676611099538</v>
       </c>
       <c r="F143" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>9</v>
       </c>
@@ -4506,7 +4558,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>10</v>
       </c>
@@ -4517,13 +4569,13 @@
         <v>297</v>
       </c>
       <c r="D145" s="2">
-        <v>43563.95673082176</v>
+        <v>43563.956730821759</v>
       </c>
       <c r="F145" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>11</v>
       </c>
@@ -4534,11 +4586,23 @@
         <v>298</v>
       </c>
       <c r="D146" s="2">
-        <v>43563.95673144676</v>
+        <v>43563.956731446757</v>
       </c>
       <c r="F146" t="s">
         <v>300</v>
       </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D147" s="2"/>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D148" s="2"/>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D149" s="2"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D150" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>